<commit_message>
cardtooltip add rate description; droprate recheck
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/HItem.xlsx
+++ b/ConfigData/Xlsx/HItem.xlsx
@@ -213,7 +213,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2832" uniqueCount="1372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2832" uniqueCount="1370">
   <si>
     <t>血蓟</t>
   </si>
@@ -3889,22 +3889,10 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>使用后获得随机卡片5张，极小概率获得高等级卡片</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>获得一张随机武器卡(战斗时使用)</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>使用后获得随机卡片5张，小概率获得高等级卡片</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>使用后获得随机卡片5张，高概率获得高等级卡片</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>随机幻兽卡</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -4515,6 +4503,10 @@
   </si>
   <si>
     <t>libaohei</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用后获得随机卡片5张</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -5364,7 +5356,14 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="54">
+  <dxfs count="55">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -6711,78 +6710,78 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:N346" totalsRowShown="0" headerRowDxfId="52" dataDxfId="51" tableBorderDxfId="50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:N346" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52" tableBorderDxfId="51">
   <autoFilter ref="A3:N346"/>
   <sortState ref="A4:O435">
     <sortCondition ref="A3:A435"/>
   </sortState>
   <tableColumns count="14">
-    <tableColumn id="1" name="Id" dataDxfId="49"/>
-    <tableColumn id="2" name="Name" dataDxfId="48"/>
-    <tableColumn id="3" name="Type" dataDxfId="47"/>
-    <tableColumn id="4" name="Descript" dataDxfId="46"/>
-    <tableColumn id="5" name="Level" dataDxfId="45"/>
-    <tableColumn id="6" name="Rare" dataDxfId="44"/>
-    <tableColumn id="7" name="MaxPile" dataDxfId="43"/>
-    <tableColumn id="8" name="Value" dataDxfId="42"/>
-    <tableColumn id="9" name="SubType" dataDxfId="41"/>
-    <tableColumn id="11" name="IsUsable" dataDxfId="40"/>
-    <tableColumn id="12" name="IsThrowable" dataDxfId="39"/>
-    <tableColumn id="15" name="IsRandom" dataDxfId="38"/>
-    <tableColumn id="13" name="CdGroup" dataDxfId="37"/>
-    <tableColumn id="14" name="Url" dataDxfId="36"/>
+    <tableColumn id="1" name="Id" dataDxfId="50"/>
+    <tableColumn id="2" name="Name" dataDxfId="49"/>
+    <tableColumn id="3" name="Type" dataDxfId="48"/>
+    <tableColumn id="4" name="Descript" dataDxfId="47"/>
+    <tableColumn id="5" name="Level" dataDxfId="46"/>
+    <tableColumn id="6" name="Rare" dataDxfId="45"/>
+    <tableColumn id="7" name="MaxPile" dataDxfId="44"/>
+    <tableColumn id="8" name="Value" dataDxfId="43"/>
+    <tableColumn id="9" name="SubType" dataDxfId="42"/>
+    <tableColumn id="11" name="IsUsable" dataDxfId="41"/>
+    <tableColumn id="12" name="IsThrowable" dataDxfId="40"/>
+    <tableColumn id="15" name="IsRandom" dataDxfId="39"/>
+    <tableColumn id="13" name="CdGroup" dataDxfId="38"/>
+    <tableColumn id="14" name="Url" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A3:N14" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33" tableBorderDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A3:N14" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34" tableBorderDxfId="33">
   <autoFilter ref="A3:N14"/>
   <sortState ref="A4:O435">
     <sortCondition ref="A3:A435"/>
   </sortState>
   <tableColumns count="14">
-    <tableColumn id="1" name="Id" dataDxfId="31"/>
-    <tableColumn id="2" name="Name" dataDxfId="30"/>
-    <tableColumn id="3" name="Type" dataDxfId="29"/>
-    <tableColumn id="4" name="Descript" dataDxfId="28"/>
-    <tableColumn id="5" name="Level" dataDxfId="27"/>
-    <tableColumn id="6" name="Rare" dataDxfId="26"/>
-    <tableColumn id="7" name="MaxPile" dataDxfId="25"/>
-    <tableColumn id="8" name="Value" dataDxfId="24"/>
-    <tableColumn id="9" name="SubType" dataDxfId="23"/>
-    <tableColumn id="11" name="IsUsable" dataDxfId="22"/>
-    <tableColumn id="12" name="IsThrowable" dataDxfId="21"/>
-    <tableColumn id="15" name="IsRandom" dataDxfId="20"/>
-    <tableColumn id="13" name="CdGroup" dataDxfId="19"/>
-    <tableColumn id="14" name="Url" dataDxfId="18"/>
+    <tableColumn id="1" name="Id" dataDxfId="32"/>
+    <tableColumn id="2" name="Name" dataDxfId="31"/>
+    <tableColumn id="3" name="Type" dataDxfId="30"/>
+    <tableColumn id="4" name="Descript" dataDxfId="29"/>
+    <tableColumn id="5" name="Level" dataDxfId="28"/>
+    <tableColumn id="6" name="Rare" dataDxfId="27"/>
+    <tableColumn id="7" name="MaxPile" dataDxfId="26"/>
+    <tableColumn id="8" name="Value" dataDxfId="25"/>
+    <tableColumn id="9" name="SubType" dataDxfId="24"/>
+    <tableColumn id="11" name="IsUsable" dataDxfId="23"/>
+    <tableColumn id="12" name="IsThrowable" dataDxfId="22"/>
+    <tableColumn id="15" name="IsRandom" dataDxfId="21"/>
+    <tableColumn id="13" name="CdGroup" dataDxfId="20"/>
+    <tableColumn id="14" name="Url" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表1_34" displayName="表1_34" ref="A3:N100" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15" tableBorderDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表1_34" displayName="表1_34" ref="A3:N100" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16" tableBorderDxfId="15">
   <autoFilter ref="A3:N100"/>
   <sortState ref="A4:O99">
     <sortCondition ref="A3:A99"/>
   </sortState>
   <tableColumns count="14">
-    <tableColumn id="1" name="Id" dataDxfId="13"/>
-    <tableColumn id="2" name="Name" dataDxfId="12"/>
-    <tableColumn id="3" name="Type" dataDxfId="11"/>
-    <tableColumn id="4" name="Descript" dataDxfId="10"/>
-    <tableColumn id="5" name="Level" dataDxfId="9"/>
-    <tableColumn id="6" name="Rare" dataDxfId="8"/>
-    <tableColumn id="7" name="MaxPile" dataDxfId="7"/>
-    <tableColumn id="8" name="Value" dataDxfId="6"/>
-    <tableColumn id="9" name="SubType" dataDxfId="5"/>
-    <tableColumn id="11" name="IsUsable" dataDxfId="4"/>
-    <tableColumn id="12" name="IsThrowable" dataDxfId="3"/>
-    <tableColumn id="15" name="IsRandom" dataDxfId="2"/>
-    <tableColumn id="13" name="CdGroup" dataDxfId="1"/>
-    <tableColumn id="14" name="Url" dataDxfId="0"/>
+    <tableColumn id="1" name="Id" dataDxfId="14"/>
+    <tableColumn id="2" name="Name" dataDxfId="13"/>
+    <tableColumn id="3" name="Type" dataDxfId="12"/>
+    <tableColumn id="4" name="Descript" dataDxfId="11"/>
+    <tableColumn id="5" name="Level" dataDxfId="10"/>
+    <tableColumn id="6" name="Rare" dataDxfId="9"/>
+    <tableColumn id="7" name="MaxPile" dataDxfId="8"/>
+    <tableColumn id="8" name="Value" dataDxfId="7"/>
+    <tableColumn id="9" name="SubType" dataDxfId="6"/>
+    <tableColumn id="11" name="IsUsable" dataDxfId="5"/>
+    <tableColumn id="12" name="IsThrowable" dataDxfId="4"/>
+    <tableColumn id="15" name="IsRandom" dataDxfId="3"/>
+    <tableColumn id="13" name="CdGroup" dataDxfId="2"/>
+    <tableColumn id="14" name="Url" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7123,7 +7122,7 @@
         <v>1179</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>1220</v>
+        <v>1217</v>
       </c>
       <c r="K1" s="5" t="s">
         <v>1181</v>
@@ -10962,13 +10961,13 @@
         <v>22011057</v>
       </c>
       <c r="B95" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="C95">
         <v>2</v>
       </c>
       <c r="D95" t="s">
-        <v>1259</v>
+        <v>1256</v>
       </c>
       <c r="E95">
         <v>1</v>
@@ -10995,7 +10994,7 @@
         <v>1202</v>
       </c>
       <c r="N95" t="s">
-        <v>1257</v>
+        <v>1254</v>
       </c>
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.25">
@@ -11577,13 +11576,13 @@
         <v>22011072</v>
       </c>
       <c r="B110" t="s">
-        <v>1260</v>
+        <v>1257</v>
       </c>
       <c r="C110">
         <v>2</v>
       </c>
       <c r="D110" t="s">
-        <v>1262</v>
+        <v>1259</v>
       </c>
       <c r="E110">
         <v>1</v>
@@ -11610,7 +11609,7 @@
         <v>1202</v>
       </c>
       <c r="N110" t="s">
-        <v>1261</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="111" spans="1:14" x14ac:dyDescent="0.25">
@@ -15226,13 +15225,13 @@
         <v>22011161</v>
       </c>
       <c r="B199" t="s">
-        <v>1263</v>
+        <v>1260</v>
       </c>
       <c r="C199">
         <v>2</v>
       </c>
       <c r="D199" t="s">
-        <v>1265</v>
+        <v>1262</v>
       </c>
       <c r="E199">
         <v>1</v>
@@ -15259,7 +15258,7 @@
         <v>1202</v>
       </c>
       <c r="N199" t="s">
-        <v>1264</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="200" spans="1:14" x14ac:dyDescent="0.25">
@@ -15997,7 +15996,7 @@
         <v>1202</v>
       </c>
       <c r="N217" t="s">
-        <v>1314</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="218" spans="1:14" x14ac:dyDescent="0.25">
@@ -16251,13 +16250,13 @@
         <v>22011186</v>
       </c>
       <c r="B224" t="s">
-        <v>1237</v>
+        <v>1234</v>
       </c>
       <c r="C224">
         <v>2</v>
       </c>
       <c r="D224" t="s">
-        <v>1238</v>
+        <v>1235</v>
       </c>
       <c r="E224">
         <v>1</v>
@@ -16284,7 +16283,7 @@
         <v>1202</v>
       </c>
       <c r="N224" t="s">
-        <v>1236</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="225" spans="1:14" x14ac:dyDescent="0.25">
@@ -16292,13 +16291,13 @@
         <v>22011187</v>
       </c>
       <c r="B225" t="s">
-        <v>1240</v>
+        <v>1237</v>
       </c>
       <c r="C225">
         <v>2</v>
       </c>
       <c r="D225" t="s">
-        <v>1241</v>
+        <v>1238</v>
       </c>
       <c r="E225">
         <v>1</v>
@@ -16325,7 +16324,7 @@
         <v>1202</v>
       </c>
       <c r="N225" t="s">
-        <v>1239</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="226" spans="1:14" x14ac:dyDescent="0.25">
@@ -16333,13 +16332,13 @@
         <v>22011188</v>
       </c>
       <c r="B226" t="s">
-        <v>1243</v>
+        <v>1240</v>
       </c>
       <c r="C226">
         <v>2</v>
       </c>
       <c r="D226" t="s">
-        <v>1244</v>
+        <v>1241</v>
       </c>
       <c r="E226">
         <v>1</v>
@@ -16366,7 +16365,7 @@
         <v>1202</v>
       </c>
       <c r="N226" t="s">
-        <v>1242</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="227" spans="1:14" x14ac:dyDescent="0.25">
@@ -16374,13 +16373,13 @@
         <v>22011189</v>
       </c>
       <c r="B227" t="s">
-        <v>1246</v>
+        <v>1243</v>
       </c>
       <c r="C227">
         <v>2</v>
       </c>
       <c r="D227" t="s">
-        <v>1247</v>
+        <v>1244</v>
       </c>
       <c r="E227">
         <v>1</v>
@@ -16407,7 +16406,7 @@
         <v>1202</v>
       </c>
       <c r="N227" t="s">
-        <v>1245</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="228" spans="1:14" x14ac:dyDescent="0.25">
@@ -16415,13 +16414,13 @@
         <v>22011190</v>
       </c>
       <c r="B228" t="s">
-        <v>1249</v>
+        <v>1246</v>
       </c>
       <c r="C228">
         <v>2</v>
       </c>
       <c r="D228" t="s">
-        <v>1250</v>
+        <v>1247</v>
       </c>
       <c r="E228">
         <v>1</v>
@@ -16449,7 +16448,7 @@
       </c>
       <c r="M228" s="19"/>
       <c r="N228" s="19" t="s">
-        <v>1248</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="229" spans="1:14" x14ac:dyDescent="0.25">
@@ -16457,13 +16456,13 @@
         <v>22011191</v>
       </c>
       <c r="B229" t="s">
-        <v>1252</v>
+        <v>1249</v>
       </c>
       <c r="C229">
         <v>2</v>
       </c>
       <c r="D229" t="s">
-        <v>1253</v>
+        <v>1250</v>
       </c>
       <c r="E229">
         <v>1</v>
@@ -16491,7 +16490,7 @@
       </c>
       <c r="M229" s="19"/>
       <c r="N229" s="19" t="s">
-        <v>1251</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="230" spans="1:14" x14ac:dyDescent="0.25">
@@ -16499,13 +16498,13 @@
         <v>22011192</v>
       </c>
       <c r="B230" t="s">
-        <v>1255</v>
+        <v>1252</v>
       </c>
       <c r="C230">
         <v>2</v>
       </c>
       <c r="D230" t="s">
-        <v>1256</v>
+        <v>1253</v>
       </c>
       <c r="E230">
         <v>1</v>
@@ -16533,7 +16532,7 @@
       </c>
       <c r="M230" s="19"/>
       <c r="N230" s="19" t="s">
-        <v>1254</v>
+        <v>1251</v>
       </c>
     </row>
     <row r="231" spans="1:14" x14ac:dyDescent="0.25">
@@ -16541,13 +16540,13 @@
         <v>22011193</v>
       </c>
       <c r="B231" t="s">
-        <v>1267</v>
+        <v>1264</v>
       </c>
       <c r="C231">
         <v>2</v>
       </c>
       <c r="D231" t="s">
-        <v>1268</v>
+        <v>1265</v>
       </c>
       <c r="E231">
         <v>1</v>
@@ -16575,7 +16574,7 @@
       </c>
       <c r="M231" s="19"/>
       <c r="N231" s="19" t="s">
-        <v>1266</v>
+        <v>1263</v>
       </c>
     </row>
     <row r="232" spans="1:14" x14ac:dyDescent="0.25">
@@ -16583,13 +16582,13 @@
         <v>22011194</v>
       </c>
       <c r="B232" t="s">
-        <v>1271</v>
+        <v>1268</v>
       </c>
       <c r="C232">
         <v>2</v>
       </c>
       <c r="D232" t="s">
-        <v>1273</v>
+        <v>1270</v>
       </c>
       <c r="E232">
         <v>1</v>
@@ -16617,7 +16616,7 @@
       </c>
       <c r="M232" s="19"/>
       <c r="N232" s="19" t="s">
-        <v>1269</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="233" spans="1:14" x14ac:dyDescent="0.25">
@@ -16625,13 +16624,13 @@
         <v>22011195</v>
       </c>
       <c r="B233" t="s">
-        <v>1272</v>
+        <v>1269</v>
       </c>
       <c r="C233">
         <v>2</v>
       </c>
       <c r="D233" t="s">
-        <v>1274</v>
+        <v>1271</v>
       </c>
       <c r="E233">
         <v>1</v>
@@ -16659,7 +16658,7 @@
       </c>
       <c r="M233" s="19"/>
       <c r="N233" s="19" t="s">
-        <v>1270</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="234" spans="1:14" x14ac:dyDescent="0.25">
@@ -16667,13 +16666,13 @@
         <v>22011196</v>
       </c>
       <c r="B234" t="s">
-        <v>1276</v>
+        <v>1273</v>
       </c>
       <c r="C234">
         <v>2</v>
       </c>
       <c r="D234" t="s">
-        <v>1277</v>
+        <v>1274</v>
       </c>
       <c r="E234">
         <v>1</v>
@@ -16701,7 +16700,7 @@
       </c>
       <c r="M234" s="19"/>
       <c r="N234" s="19" t="s">
-        <v>1275</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="235" spans="1:14" x14ac:dyDescent="0.25">
@@ -16709,13 +16708,13 @@
         <v>22011197</v>
       </c>
       <c r="B235" t="s">
-        <v>1279</v>
+        <v>1276</v>
       </c>
       <c r="C235">
         <v>2</v>
       </c>
       <c r="D235" t="s">
-        <v>1280</v>
+        <v>1277</v>
       </c>
       <c r="E235">
         <v>1</v>
@@ -16743,7 +16742,7 @@
       </c>
       <c r="M235" s="19"/>
       <c r="N235" s="19" t="s">
-        <v>1278</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="236" spans="1:14" x14ac:dyDescent="0.25">
@@ -16751,13 +16750,13 @@
         <v>22011198</v>
       </c>
       <c r="B236" t="s">
-        <v>1282</v>
+        <v>1279</v>
       </c>
       <c r="C236">
         <v>2</v>
       </c>
       <c r="D236" t="s">
-        <v>1283</v>
+        <v>1280</v>
       </c>
       <c r="E236">
         <v>1</v>
@@ -16785,7 +16784,7 @@
       </c>
       <c r="M236" s="19"/>
       <c r="N236" s="19" t="s">
-        <v>1281</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="237" spans="1:14" x14ac:dyDescent="0.25">
@@ -16793,13 +16792,13 @@
         <v>22011199</v>
       </c>
       <c r="B237" t="s">
-        <v>1285</v>
+        <v>1282</v>
       </c>
       <c r="C237">
         <v>2</v>
       </c>
       <c r="D237" t="s">
-        <v>1286</v>
+        <v>1283</v>
       </c>
       <c r="E237">
         <v>1</v>
@@ -16827,7 +16826,7 @@
       </c>
       <c r="M237" s="19"/>
       <c r="N237" s="19" t="s">
-        <v>1284</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="238" spans="1:14" x14ac:dyDescent="0.25">
@@ -16835,13 +16834,13 @@
         <v>22011200</v>
       </c>
       <c r="B238" t="s">
-        <v>1288</v>
+        <v>1285</v>
       </c>
       <c r="C238">
         <v>2</v>
       </c>
       <c r="D238" t="s">
-        <v>1289</v>
+        <v>1286</v>
       </c>
       <c r="E238">
         <v>1</v>
@@ -16869,7 +16868,7 @@
       </c>
       <c r="M238" s="19"/>
       <c r="N238" s="19" t="s">
-        <v>1287</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="239" spans="1:14" x14ac:dyDescent="0.25">
@@ -16877,13 +16876,13 @@
         <v>22011201</v>
       </c>
       <c r="B239" t="s">
-        <v>1345</v>
+        <v>1342</v>
       </c>
       <c r="C239">
         <v>2</v>
       </c>
       <c r="D239" t="s">
-        <v>1347</v>
+        <v>1344</v>
       </c>
       <c r="E239">
         <v>1</v>
@@ -16911,7 +16910,7 @@
       </c>
       <c r="M239" s="19"/>
       <c r="N239" s="19" t="s">
-        <v>1346</v>
+        <v>1343</v>
       </c>
     </row>
     <row r="240" spans="1:14" x14ac:dyDescent="0.25">
@@ -16919,13 +16918,13 @@
         <v>22011202</v>
       </c>
       <c r="B240" t="s">
-        <v>1291</v>
+        <v>1288</v>
       </c>
       <c r="C240">
         <v>2</v>
       </c>
       <c r="D240" t="s">
-        <v>1292</v>
+        <v>1289</v>
       </c>
       <c r="E240">
         <v>1</v>
@@ -16953,7 +16952,7 @@
       </c>
       <c r="M240" s="19"/>
       <c r="N240" s="19" t="s">
-        <v>1290</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="241" spans="1:14" x14ac:dyDescent="0.25">
@@ -16961,13 +16960,13 @@
         <v>22011203</v>
       </c>
       <c r="B241" t="s">
-        <v>1294</v>
+        <v>1291</v>
       </c>
       <c r="C241">
         <v>2</v>
       </c>
       <c r="D241" t="s">
-        <v>1295</v>
+        <v>1292</v>
       </c>
       <c r="E241">
         <v>1</v>
@@ -16995,7 +16994,7 @@
       </c>
       <c r="M241" s="19"/>
       <c r="N241" s="19" t="s">
-        <v>1293</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="242" spans="1:14" x14ac:dyDescent="0.25">
@@ -17003,13 +17002,13 @@
         <v>22011204</v>
       </c>
       <c r="B242" t="s">
-        <v>1297</v>
+        <v>1294</v>
       </c>
       <c r="C242">
         <v>2</v>
       </c>
       <c r="D242" t="s">
-        <v>1298</v>
+        <v>1295</v>
       </c>
       <c r="E242">
         <v>1</v>
@@ -17037,7 +17036,7 @@
       </c>
       <c r="M242" s="19"/>
       <c r="N242" s="19" t="s">
-        <v>1296</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="243" spans="1:14" x14ac:dyDescent="0.25">
@@ -17045,13 +17044,13 @@
         <v>22011205</v>
       </c>
       <c r="B243" t="s">
-        <v>1300</v>
+        <v>1297</v>
       </c>
       <c r="C243">
         <v>2</v>
       </c>
       <c r="D243" t="s">
-        <v>1301</v>
+        <v>1298</v>
       </c>
       <c r="E243">
         <v>1</v>
@@ -17079,7 +17078,7 @@
       </c>
       <c r="M243" s="19"/>
       <c r="N243" s="19" t="s">
-        <v>1299</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="244" spans="1:14" x14ac:dyDescent="0.25">
@@ -17087,13 +17086,13 @@
         <v>22011206</v>
       </c>
       <c r="B244" t="s">
-        <v>1303</v>
+        <v>1300</v>
       </c>
       <c r="C244">
         <v>2</v>
       </c>
       <c r="D244" t="s">
-        <v>1304</v>
+        <v>1301</v>
       </c>
       <c r="E244">
         <v>1</v>
@@ -17121,7 +17120,7 @@
       </c>
       <c r="M244" s="19"/>
       <c r="N244" s="19" t="s">
-        <v>1302</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="245" spans="1:14" x14ac:dyDescent="0.25">
@@ -17129,13 +17128,13 @@
         <v>22011207</v>
       </c>
       <c r="B245" t="s">
-        <v>1306</v>
+        <v>1303</v>
       </c>
       <c r="C245">
         <v>2</v>
       </c>
       <c r="D245" t="s">
-        <v>1307</v>
+        <v>1304</v>
       </c>
       <c r="E245">
         <v>1</v>
@@ -17163,7 +17162,7 @@
       </c>
       <c r="M245" s="19"/>
       <c r="N245" s="19" t="s">
-        <v>1305</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="246" spans="1:14" x14ac:dyDescent="0.25">
@@ -17171,13 +17170,13 @@
         <v>22011208</v>
       </c>
       <c r="B246" t="s">
-        <v>1309</v>
+        <v>1306</v>
       </c>
       <c r="C246">
         <v>2</v>
       </c>
       <c r="D246" t="s">
-        <v>1310</v>
+        <v>1307</v>
       </c>
       <c r="E246">
         <v>1</v>
@@ -17205,7 +17204,7 @@
       </c>
       <c r="M246" s="19"/>
       <c r="N246" s="19" t="s">
-        <v>1308</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="247" spans="1:14" x14ac:dyDescent="0.25">
@@ -17213,13 +17212,13 @@
         <v>22011209</v>
       </c>
       <c r="B247" t="s">
-        <v>1312</v>
+        <v>1309</v>
       </c>
       <c r="C247">
         <v>2</v>
       </c>
       <c r="D247" t="s">
-        <v>1313</v>
+        <v>1310</v>
       </c>
       <c r="E247">
         <v>1</v>
@@ -17247,7 +17246,7 @@
       </c>
       <c r="M247" s="19"/>
       <c r="N247" s="19" t="s">
-        <v>1311</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="248" spans="1:14" x14ac:dyDescent="0.25">
@@ -17255,13 +17254,13 @@
         <v>22011210</v>
       </c>
       <c r="B248" t="s">
-        <v>1315</v>
+        <v>1312</v>
       </c>
       <c r="C248">
         <v>2</v>
       </c>
       <c r="D248" t="s">
-        <v>1316</v>
+        <v>1313</v>
       </c>
       <c r="E248">
         <v>1</v>
@@ -17289,7 +17288,7 @@
       </c>
       <c r="M248" s="19"/>
       <c r="N248" s="19" t="s">
-        <v>1335</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="249" spans="1:14" x14ac:dyDescent="0.25">
@@ -17297,13 +17296,13 @@
         <v>22011211</v>
       </c>
       <c r="B249" t="s">
-        <v>1318</v>
+        <v>1315</v>
       </c>
       <c r="C249">
         <v>2</v>
       </c>
       <c r="D249" t="s">
-        <v>1319</v>
+        <v>1316</v>
       </c>
       <c r="E249">
         <v>1</v>
@@ -17331,7 +17330,7 @@
       </c>
       <c r="M249" s="19"/>
       <c r="N249" s="19" t="s">
-        <v>1317</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="250" spans="1:14" x14ac:dyDescent="0.25">
@@ -17339,13 +17338,13 @@
         <v>22011212</v>
       </c>
       <c r="B250" t="s">
-        <v>1321</v>
+        <v>1318</v>
       </c>
       <c r="C250">
         <v>2</v>
       </c>
       <c r="D250" t="s">
-        <v>1322</v>
+        <v>1319</v>
       </c>
       <c r="E250">
         <v>1</v>
@@ -17373,7 +17372,7 @@
       </c>
       <c r="M250" s="19"/>
       <c r="N250" s="19" t="s">
-        <v>1320</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="251" spans="1:14" x14ac:dyDescent="0.25">
@@ -17381,13 +17380,13 @@
         <v>22011213</v>
       </c>
       <c r="B251" t="s">
-        <v>1324</v>
+        <v>1321</v>
       </c>
       <c r="C251">
         <v>2</v>
       </c>
       <c r="D251" t="s">
-        <v>1325</v>
+        <v>1322</v>
       </c>
       <c r="E251">
         <v>1</v>
@@ -17415,7 +17414,7 @@
       </c>
       <c r="M251" s="19"/>
       <c r="N251" s="19" t="s">
-        <v>1323</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="252" spans="1:14" x14ac:dyDescent="0.25">
@@ -17423,13 +17422,13 @@
         <v>22011214</v>
       </c>
       <c r="B252" t="s">
-        <v>1327</v>
+        <v>1324</v>
       </c>
       <c r="C252">
         <v>2</v>
       </c>
       <c r="D252" t="s">
-        <v>1328</v>
+        <v>1325</v>
       </c>
       <c r="E252">
         <v>1</v>
@@ -17457,7 +17456,7 @@
       </c>
       <c r="M252" s="19"/>
       <c r="N252" s="19" t="s">
-        <v>1326</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="253" spans="1:14" x14ac:dyDescent="0.25">
@@ -17465,13 +17464,13 @@
         <v>22011215</v>
       </c>
       <c r="B253" t="s">
-        <v>1330</v>
+        <v>1327</v>
       </c>
       <c r="C253">
         <v>2</v>
       </c>
       <c r="D253" t="s">
-        <v>1331</v>
+        <v>1328</v>
       </c>
       <c r="E253">
         <v>1</v>
@@ -17499,7 +17498,7 @@
       </c>
       <c r="M253" s="19"/>
       <c r="N253" s="19" t="s">
-        <v>1329</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="254" spans="1:14" x14ac:dyDescent="0.25">
@@ -17507,13 +17506,13 @@
         <v>22011216</v>
       </c>
       <c r="B254" t="s">
-        <v>1332</v>
+        <v>1329</v>
       </c>
       <c r="C254">
         <v>2</v>
       </c>
       <c r="D254" t="s">
-        <v>1333</v>
+        <v>1330</v>
       </c>
       <c r="E254">
         <v>1</v>
@@ -17549,13 +17548,13 @@
         <v>22011217</v>
       </c>
       <c r="B255" t="s">
-        <v>1336</v>
+        <v>1333</v>
       </c>
       <c r="C255">
         <v>2</v>
       </c>
       <c r="D255" t="s">
-        <v>1337</v>
+        <v>1334</v>
       </c>
       <c r="E255">
         <v>1</v>
@@ -17583,7 +17582,7 @@
       </c>
       <c r="M255" s="19"/>
       <c r="N255" s="19" t="s">
-        <v>1334</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="256" spans="1:14" x14ac:dyDescent="0.25">
@@ -17591,13 +17590,13 @@
         <v>22011218</v>
       </c>
       <c r="B256" t="s">
-        <v>1339</v>
+        <v>1336</v>
       </c>
       <c r="C256">
         <v>2</v>
       </c>
       <c r="D256" t="s">
-        <v>1340</v>
+        <v>1337</v>
       </c>
       <c r="E256">
         <v>1</v>
@@ -17625,7 +17624,7 @@
       </c>
       <c r="M256" s="19"/>
       <c r="N256" s="19" t="s">
-        <v>1338</v>
+        <v>1335</v>
       </c>
     </row>
     <row r="257" spans="1:14" x14ac:dyDescent="0.25">
@@ -17633,13 +17632,13 @@
         <v>22011219</v>
       </c>
       <c r="B257" t="s">
-        <v>1343</v>
+        <v>1340</v>
       </c>
       <c r="C257">
         <v>2</v>
       </c>
       <c r="D257" t="s">
-        <v>1342</v>
+        <v>1339</v>
       </c>
       <c r="E257">
         <v>1</v>
@@ -17666,7 +17665,7 @@
         <v>1202</v>
       </c>
       <c r="N257" t="s">
-        <v>1341</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="258" spans="1:14" x14ac:dyDescent="0.25">
@@ -17674,13 +17673,13 @@
         <v>22011220</v>
       </c>
       <c r="B258" t="s">
-        <v>1349</v>
+        <v>1346</v>
       </c>
       <c r="C258">
         <v>2</v>
       </c>
       <c r="D258" t="s">
-        <v>1350</v>
+        <v>1347</v>
       </c>
       <c r="E258">
         <v>1</v>
@@ -17707,7 +17706,7 @@
         <v>1202</v>
       </c>
       <c r="N258" t="s">
-        <v>1348</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="259" spans="1:14" x14ac:dyDescent="0.25">
@@ -17715,13 +17714,13 @@
         <v>22011221</v>
       </c>
       <c r="B259" t="s">
-        <v>1352</v>
+        <v>1349</v>
       </c>
       <c r="C259">
         <v>2</v>
       </c>
       <c r="D259" t="s">
-        <v>1353</v>
+        <v>1350</v>
       </c>
       <c r="E259">
         <v>1</v>
@@ -17748,7 +17747,7 @@
         <v>1202</v>
       </c>
       <c r="N259" t="s">
-        <v>1351</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="260" spans="1:14" x14ac:dyDescent="0.25">
@@ -18878,7 +18877,7 @@
         <v>1202</v>
       </c>
       <c r="N287" t="s">
-        <v>1344</v>
+        <v>1341</v>
       </c>
     </row>
     <row r="288" spans="1:14" x14ac:dyDescent="0.25">
@@ -21303,7 +21302,7 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="A4:N346">
-    <cfRule type="containsBlanks" dxfId="53" priority="1">
+    <cfRule type="containsBlanks" dxfId="54" priority="1">
       <formula>LEN(TRIM(A4))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21528,7 +21527,7 @@
         <v>3</v>
       </c>
       <c r="J5" t="s">
-        <v>1219</v>
+        <v>1216</v>
       </c>
       <c r="K5" t="s">
         <v>1203</v>
@@ -21876,7 +21875,7 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="A4:N14">
-    <cfRule type="containsBlanks" dxfId="35" priority="1">
+    <cfRule type="containsBlanks" dxfId="36" priority="1">
       <formula>LEN(TRIM(A4))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21894,10 +21893,10 @@
   <dimension ref="A1:N100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B49" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="N11" sqref="N11"/>
+      <selection pane="bottomRight" activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -22075,7 +22074,7 @@
         <v>1203</v>
       </c>
       <c r="L4" t="s">
-        <v>1225</v>
+        <v>1222</v>
       </c>
       <c r="N4" t="s">
         <v>927</v>
@@ -22086,13 +22085,13 @@
         <v>22031002</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>1355</v>
+        <v>1352</v>
       </c>
       <c r="C5" s="7">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>1362</v>
+        <v>1359</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -22107,7 +22106,7 @@
         <v>50</v>
       </c>
       <c r="I5">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J5" t="s">
         <v>1201</v>
@@ -22116,7 +22115,7 @@
         <v>1203</v>
       </c>
       <c r="L5" t="s">
-        <v>1225</v>
+        <v>1222</v>
       </c>
       <c r="N5" t="s">
         <v>928</v>
@@ -22127,13 +22126,13 @@
         <v>22031003</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>1356</v>
+        <v>1353</v>
       </c>
       <c r="C6" s="7">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>1363</v>
+        <v>1360</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -22148,7 +22147,7 @@
         <v>50</v>
       </c>
       <c r="I6">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J6" t="s">
         <v>1201</v>
@@ -22157,7 +22156,7 @@
         <v>1203</v>
       </c>
       <c r="L6" t="s">
-        <v>1225</v>
+        <v>1222</v>
       </c>
       <c r="N6" t="s">
         <v>929</v>
@@ -22168,13 +22167,13 @@
         <v>22031004</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>1357</v>
+        <v>1354</v>
       </c>
       <c r="C7" s="7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>1364</v>
+        <v>1361</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -22189,16 +22188,16 @@
         <v>50</v>
       </c>
       <c r="I7">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J7" t="s">
-        <v>1226</v>
+        <v>1223</v>
       </c>
       <c r="K7" t="s">
         <v>1203</v>
       </c>
       <c r="L7" t="s">
-        <v>1225</v>
+        <v>1222</v>
       </c>
       <c r="N7" t="s">
         <v>930</v>
@@ -22209,13 +22208,13 @@
         <v>22031005</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>1358</v>
+        <v>1355</v>
       </c>
       <c r="C8" s="7">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>1365</v>
+        <v>1362</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -22230,7 +22229,7 @@
         <v>50</v>
       </c>
       <c r="I8">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J8" t="s">
         <v>1201</v>
@@ -22239,7 +22238,7 @@
         <v>1203</v>
       </c>
       <c r="L8" t="s">
-        <v>1225</v>
+        <v>1222</v>
       </c>
       <c r="N8" t="s">
         <v>931</v>
@@ -22250,13 +22249,13 @@
         <v>22031006</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>1359</v>
+        <v>1356</v>
       </c>
       <c r="C9" s="7">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>1366</v>
+        <v>1363</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -22271,7 +22270,7 @@
         <v>50</v>
       </c>
       <c r="I9">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J9" t="s">
         <v>1201</v>
@@ -22280,10 +22279,10 @@
         <v>1203</v>
       </c>
       <c r="L9" t="s">
-        <v>1225</v>
+        <v>1222</v>
       </c>
       <c r="N9" t="s">
-        <v>1369</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -22291,13 +22290,13 @@
         <v>22031007</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>1360</v>
+        <v>1357</v>
       </c>
       <c r="C10" s="7">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>1367</v>
+        <v>1364</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -22312,7 +22311,7 @@
         <v>50</v>
       </c>
       <c r="I10">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J10" t="s">
         <v>1201</v>
@@ -22321,10 +22320,10 @@
         <v>1203</v>
       </c>
       <c r="L10" t="s">
-        <v>1225</v>
+        <v>1222</v>
       </c>
       <c r="N10" t="s">
-        <v>1370</v>
+        <v>1367</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -22332,13 +22331,13 @@
         <v>22031008</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>1361</v>
+        <v>1358</v>
       </c>
       <c r="C11" s="7">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>1368</v>
+        <v>1365</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -22353,7 +22352,7 @@
         <v>50</v>
       </c>
       <c r="I11">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J11" t="s">
         <v>1201</v>
@@ -22362,10 +22361,10 @@
         <v>1203</v>
       </c>
       <c r="L11" t="s">
-        <v>1225</v>
+        <v>1222</v>
       </c>
       <c r="N11" t="s">
-        <v>1371</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -22403,7 +22402,7 @@
         <v>1203</v>
       </c>
       <c r="L12" t="s">
-        <v>1225</v>
+        <v>1222</v>
       </c>
       <c r="N12" t="s">
         <v>934</v>
@@ -22444,7 +22443,7 @@
         <v>1203</v>
       </c>
       <c r="L13" t="s">
-        <v>1225</v>
+        <v>1222</v>
       </c>
       <c r="N13" t="s">
         <v>937</v>
@@ -22485,7 +22484,7 @@
         <v>1203</v>
       </c>
       <c r="L14" t="s">
-        <v>1225</v>
+        <v>1222</v>
       </c>
       <c r="N14" t="s">
         <v>940</v>
@@ -22502,7 +22501,7 @@
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>1354</v>
+        <v>1351</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -22523,7 +22522,7 @@
         <v>1203</v>
       </c>
       <c r="L15" t="s">
-        <v>1225</v>
+        <v>1222</v>
       </c>
       <c r="N15" t="s">
         <v>942</v>
@@ -22561,7 +22560,7 @@
         <v>1203</v>
       </c>
       <c r="L16" t="s">
-        <v>1225</v>
+        <v>1222</v>
       </c>
       <c r="N16" t="s">
         <v>945</v>
@@ -22599,7 +22598,7 @@
         <v>1203</v>
       </c>
       <c r="L17" t="s">
-        <v>1225</v>
+        <v>1222</v>
       </c>
       <c r="N17" t="s">
         <v>948</v>
@@ -22616,7 +22615,7 @@
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>1235</v>
+        <v>1232</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -22640,7 +22639,7 @@
         <v>1201</v>
       </c>
       <c r="L18" t="s">
-        <v>1225</v>
+        <v>1222</v>
       </c>
       <c r="N18" t="s">
         <v>950</v>
@@ -22657,7 +22656,7 @@
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>1234</v>
+        <v>1231</v>
       </c>
       <c r="E19">
         <v>1</v>
@@ -22681,7 +22680,7 @@
         <v>1201</v>
       </c>
       <c r="L19" t="s">
-        <v>1225</v>
+        <v>1222</v>
       </c>
       <c r="N19" t="s">
         <v>952</v>
@@ -22698,7 +22697,7 @@
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>1230</v>
+        <v>1227</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -22722,7 +22721,7 @@
         <v>1201</v>
       </c>
       <c r="L20" t="s">
-        <v>1225</v>
+        <v>1222</v>
       </c>
       <c r="N20" t="s">
         <v>954</v>
@@ -22739,7 +22738,7 @@
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>1231</v>
+        <v>1228</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -22763,7 +22762,7 @@
         <v>1201</v>
       </c>
       <c r="L21" t="s">
-        <v>1225</v>
+        <v>1222</v>
       </c>
       <c r="N21" t="s">
         <v>956</v>
@@ -22780,7 +22779,7 @@
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>1232</v>
+        <v>1229</v>
       </c>
       <c r="E22">
         <v>1</v>
@@ -22821,7 +22820,7 @@
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>1233</v>
+        <v>1230</v>
       </c>
       <c r="E23">
         <v>1</v>
@@ -22897,13 +22896,13 @@
         <v>22032008</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>1229</v>
+        <v>1226</v>
       </c>
       <c r="C25" s="7">
         <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>1228</v>
+        <v>1225</v>
       </c>
       <c r="E25">
         <v>1</v>
@@ -22930,7 +22929,7 @@
         <v>1204</v>
       </c>
       <c r="N25" t="s">
-        <v>1227</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
@@ -22968,7 +22967,7 @@
         <v>1201</v>
       </c>
       <c r="L26" t="s">
-        <v>1223</v>
+        <v>1220</v>
       </c>
       <c r="M26">
         <v>2</v>
@@ -23012,7 +23011,7 @@
         <v>1201</v>
       </c>
       <c r="L27" t="s">
-        <v>1223</v>
+        <v>1220</v>
       </c>
       <c r="M27">
         <v>2</v>
@@ -23056,7 +23055,7 @@
         <v>1201</v>
       </c>
       <c r="L28" t="s">
-        <v>1223</v>
+        <v>1220</v>
       </c>
       <c r="M28">
         <v>2</v>
@@ -23100,7 +23099,7 @@
         <v>1201</v>
       </c>
       <c r="L29" t="s">
-        <v>1223</v>
+        <v>1220</v>
       </c>
       <c r="M29">
         <v>3</v>
@@ -23144,7 +23143,7 @@
         <v>1201</v>
       </c>
       <c r="L30" t="s">
-        <v>1223</v>
+        <v>1220</v>
       </c>
       <c r="M30">
         <v>3</v>
@@ -23188,7 +23187,7 @@
         <v>1201</v>
       </c>
       <c r="L31" t="s">
-        <v>1223</v>
+        <v>1220</v>
       </c>
       <c r="M31">
         <v>3</v>
@@ -23232,7 +23231,7 @@
         <v>1201</v>
       </c>
       <c r="L32" t="s">
-        <v>1223</v>
+        <v>1220</v>
       </c>
       <c r="M32">
         <v>1</v>
@@ -23276,7 +23275,7 @@
         <v>1201</v>
       </c>
       <c r="L33" t="s">
-        <v>1223</v>
+        <v>1220</v>
       </c>
       <c r="M33">
         <v>1</v>
@@ -23320,7 +23319,7 @@
         <v>1201</v>
       </c>
       <c r="L34" t="s">
-        <v>1223</v>
+        <v>1220</v>
       </c>
       <c r="M34">
         <v>1</v>
@@ -23334,7 +23333,7 @@
         <v>22033013</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>1218</v>
+        <v>1215</v>
       </c>
       <c r="C35" s="7">
         <v>1</v>
@@ -23364,7 +23363,7 @@
         <v>1201</v>
       </c>
       <c r="L35" t="s">
-        <v>1223</v>
+        <v>1220</v>
       </c>
       <c r="M35">
         <v>1</v>
@@ -23384,7 +23383,7 @@
         <v>1</v>
       </c>
       <c r="D36" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="E36">
         <v>1</v>
@@ -23408,7 +23407,7 @@
         <v>1201</v>
       </c>
       <c r="L36" t="s">
-        <v>1223</v>
+        <v>1220</v>
       </c>
       <c r="M36">
         <v>4</v>
@@ -23452,7 +23451,7 @@
         <v>1201</v>
       </c>
       <c r="L37" t="s">
-        <v>1223</v>
+        <v>1220</v>
       </c>
       <c r="M37">
         <v>4</v>
@@ -23490,13 +23489,13 @@
         <v>11</v>
       </c>
       <c r="J38" t="s">
-        <v>1224</v>
+        <v>1221</v>
       </c>
       <c r="K38" t="s">
         <v>1201</v>
       </c>
       <c r="L38" t="s">
-        <v>1225</v>
+        <v>1222</v>
       </c>
       <c r="M38">
         <v>4</v>
@@ -23540,7 +23539,7 @@
         <v>1201</v>
       </c>
       <c r="L39" t="s">
-        <v>1225</v>
+        <v>1222</v>
       </c>
       <c r="M39">
         <v>4</v>
@@ -23584,7 +23583,7 @@
         <v>1201</v>
       </c>
       <c r="L40" t="s">
-        <v>1225</v>
+        <v>1222</v>
       </c>
       <c r="M40">
         <v>4</v>
@@ -23628,7 +23627,7 @@
         <v>1201</v>
       </c>
       <c r="L41" t="s">
-        <v>1225</v>
+        <v>1222</v>
       </c>
       <c r="M41">
         <v>1</v>
@@ -23672,7 +23671,7 @@
         <v>1201</v>
       </c>
       <c r="L42" t="s">
-        <v>1225</v>
+        <v>1222</v>
       </c>
       <c r="M42">
         <v>1</v>
@@ -23716,7 +23715,7 @@
         <v>1201</v>
       </c>
       <c r="L43" t="s">
-        <v>1225</v>
+        <v>1222</v>
       </c>
       <c r="M43">
         <v>1</v>
@@ -23754,13 +23753,13 @@
         <v>13</v>
       </c>
       <c r="J44" t="s">
-        <v>1226</v>
+        <v>1223</v>
       </c>
       <c r="K44" t="s">
         <v>1201</v>
       </c>
       <c r="L44" t="s">
-        <v>1225</v>
+        <v>1222</v>
       </c>
       <c r="N44" t="s">
         <v>1006</v>
@@ -23801,7 +23800,7 @@
         <v>1201</v>
       </c>
       <c r="L45" t="s">
-        <v>1225</v>
+        <v>1222</v>
       </c>
       <c r="N45" t="s">
         <v>1009</v>
@@ -23842,7 +23841,7 @@
         <v>1201</v>
       </c>
       <c r="L46" t="s">
-        <v>1225</v>
+        <v>1222</v>
       </c>
       <c r="N46" t="s">
         <v>1012</v>
@@ -23883,7 +23882,7 @@
         <v>1201</v>
       </c>
       <c r="L47" t="s">
-        <v>1225</v>
+        <v>1222</v>
       </c>
       <c r="N47" t="s">
         <v>1015</v>
@@ -23924,7 +23923,7 @@
         <v>1201</v>
       </c>
       <c r="L48" t="s">
-        <v>1225</v>
+        <v>1222</v>
       </c>
       <c r="N48" t="s">
         <v>1018</v>
@@ -23965,7 +23964,7 @@
         <v>1201</v>
       </c>
       <c r="L49" t="s">
-        <v>1225</v>
+        <v>1222</v>
       </c>
       <c r="N49" t="s">
         <v>1021</v>
@@ -24006,7 +24005,7 @@
         <v>1201</v>
       </c>
       <c r="L50" t="s">
-        <v>1225</v>
+        <v>1222</v>
       </c>
       <c r="N50" t="s">
         <v>1024</v>
@@ -24047,7 +24046,7 @@
         <v>1201</v>
       </c>
       <c r="L51" t="s">
-        <v>1225</v>
+        <v>1222</v>
       </c>
       <c r="N51" t="s">
         <v>1027</v>
@@ -24088,7 +24087,7 @@
         <v>1201</v>
       </c>
       <c r="L52" t="s">
-        <v>1225</v>
+        <v>1222</v>
       </c>
       <c r="N52" t="s">
         <v>1030</v>
@@ -24129,7 +24128,7 @@
         <v>1201</v>
       </c>
       <c r="L53" t="s">
-        <v>1225</v>
+        <v>1222</v>
       </c>
       <c r="N53" t="s">
         <v>1033</v>
@@ -24170,7 +24169,7 @@
         <v>1201</v>
       </c>
       <c r="L54" t="s">
-        <v>1225</v>
+        <v>1222</v>
       </c>
       <c r="N54" t="s">
         <v>1036</v>
@@ -24187,7 +24186,7 @@
         <v>1</v>
       </c>
       <c r="D55" t="s">
-        <v>1214</v>
+        <v>1369</v>
       </c>
       <c r="E55">
         <v>1</v>
@@ -24228,7 +24227,7 @@
         <v>1</v>
       </c>
       <c r="D56" t="s">
-        <v>1216</v>
+        <v>1369</v>
       </c>
       <c r="E56">
         <v>1</v>
@@ -24269,7 +24268,7 @@
         <v>1</v>
       </c>
       <c r="D57" t="s">
-        <v>1217</v>
+        <v>1369</v>
       </c>
       <c r="E57">
         <v>1</v>
@@ -25702,13 +25701,13 @@
         <v>13</v>
       </c>
       <c r="J97" t="s">
-        <v>1226</v>
+        <v>1223</v>
       </c>
       <c r="K97" t="s">
         <v>1201</v>
       </c>
       <c r="L97" t="s">
-        <v>1225</v>
+        <v>1222</v>
       </c>
       <c r="N97" t="s">
         <v>1162</v>
@@ -25763,7 +25762,7 @@
         <v>1</v>
       </c>
       <c r="D99" t="s">
-        <v>1221</v>
+        <v>1218</v>
       </c>
       <c r="E99">
         <v>1</v>
@@ -25784,7 +25783,7 @@
         <v>1201</v>
       </c>
       <c r="L99" t="s">
-        <v>1225</v>
+        <v>1222</v>
       </c>
       <c r="M99">
         <v>1</v>
@@ -25804,7 +25803,7 @@
         <v>1</v>
       </c>
       <c r="D100" t="s">
-        <v>1222</v>
+        <v>1219</v>
       </c>
       <c r="E100">
         <v>1</v>
@@ -25825,7 +25824,7 @@
         <v>1201</v>
       </c>
       <c r="L100" t="s">
-        <v>1225</v>
+        <v>1222</v>
       </c>
       <c r="M100">
         <v>2</v>
@@ -25837,7 +25836,7 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="D4:N100">
-    <cfRule type="containsBlanks" dxfId="17" priority="1">
+    <cfRule type="containsBlanks" dxfId="18" priority="1">
       <formula>LEN(TRIM(D4))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
add a flag attrb to the scene pos
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/HItem.xlsx
+++ b/ConfigData/Xlsx/HItem.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17766"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,7 +16,7 @@
     <sheet name="任务" sheetId="3" r:id="rId2"/>
     <sheet name="其他" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -213,7 +213,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2401" uniqueCount="1384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2406" uniqueCount="1387">
   <si>
     <t>血蓟</t>
   </si>
@@ -4617,13 +4617,25 @@
   </si>
   <si>
     <t>蓝色胶囊</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>fuwen2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>符文-卡斯</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用后可以看到本场景的所有事件</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -5471,49 +5483,7 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="63">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="57">
     <dxf>
       <fill>
         <patternFill>
@@ -6869,74 +6839,6 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -6949,92 +6851,92 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:N347" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61" tableBorderDxfId="60">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:N347" totalsRowShown="0" headerRowDxfId="56" dataDxfId="55" tableBorderDxfId="54">
   <autoFilter ref="A3:N347"/>
   <sortState ref="A4:N342">
     <sortCondition ref="A3:A342"/>
   </sortState>
   <tableColumns count="14">
-    <tableColumn id="1" name="Id" dataDxfId="59"/>
-    <tableColumn id="2" name="Name" dataDxfId="58"/>
-    <tableColumn id="3" name="Type" dataDxfId="57"/>
-    <tableColumn id="4" name="Descript" dataDxfId="56"/>
-    <tableColumn id="5" name="Level" dataDxfId="55"/>
-    <tableColumn id="6" name="Rare" dataDxfId="54"/>
-    <tableColumn id="7" name="MaxPile" dataDxfId="53"/>
-    <tableColumn id="8" name="ValueFactor" dataDxfId="52"/>
-    <tableColumn id="9" name="SubType" dataDxfId="51"/>
-    <tableColumn id="11" name="IsUsable" dataDxfId="50"/>
-    <tableColumn id="12" name="IsThrowable" dataDxfId="49"/>
-    <tableColumn id="15" name="RandomGroup" dataDxfId="48"/>
-    <tableColumn id="13" name="CdGroup" dataDxfId="47"/>
-    <tableColumn id="14" name="Url" dataDxfId="46"/>
+    <tableColumn id="1" name="Id" dataDxfId="53"/>
+    <tableColumn id="2" name="Name" dataDxfId="52"/>
+    <tableColumn id="3" name="Type" dataDxfId="51"/>
+    <tableColumn id="4" name="Descript" dataDxfId="50"/>
+    <tableColumn id="5" name="Level" dataDxfId="49"/>
+    <tableColumn id="6" name="Rare" dataDxfId="48"/>
+    <tableColumn id="7" name="MaxPile" dataDxfId="47"/>
+    <tableColumn id="8" name="ValueFactor" dataDxfId="46"/>
+    <tableColumn id="9" name="SubType" dataDxfId="45"/>
+    <tableColumn id="11" name="IsUsable" dataDxfId="44"/>
+    <tableColumn id="12" name="IsThrowable" dataDxfId="43"/>
+    <tableColumn id="15" name="RandomGroup" dataDxfId="42"/>
+    <tableColumn id="13" name="CdGroup" dataDxfId="41"/>
+    <tableColumn id="14" name="Url" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A3:N20" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44" tableBorderDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A3:N20" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38" tableBorderDxfId="37">
   <autoFilter ref="A3:N20"/>
   <sortState ref="A4:O435">
     <sortCondition ref="A3:A435"/>
   </sortState>
   <tableColumns count="14">
-    <tableColumn id="1" name="Id" dataDxfId="42"/>
-    <tableColumn id="2" name="Name" dataDxfId="41"/>
-    <tableColumn id="3" name="Type" dataDxfId="40"/>
-    <tableColumn id="4" name="Descript" dataDxfId="39"/>
-    <tableColumn id="5" name="Level" dataDxfId="38"/>
-    <tableColumn id="6" name="Rare" dataDxfId="37"/>
-    <tableColumn id="7" name="MaxPile" dataDxfId="36"/>
-    <tableColumn id="8" name="ValueFactor" dataDxfId="35"/>
-    <tableColumn id="9" name="SubType" dataDxfId="34"/>
-    <tableColumn id="11" name="IsUsable" dataDxfId="33"/>
-    <tableColumn id="12" name="IsThrowable" dataDxfId="32"/>
-    <tableColumn id="15" name="RandomGroup" dataDxfId="31"/>
-    <tableColumn id="13" name="CdGroup" dataDxfId="30"/>
-    <tableColumn id="14" name="Url" dataDxfId="29"/>
+    <tableColumn id="1" name="Id" dataDxfId="36"/>
+    <tableColumn id="2" name="Name" dataDxfId="35"/>
+    <tableColumn id="3" name="Type" dataDxfId="34"/>
+    <tableColumn id="4" name="Descript" dataDxfId="33"/>
+    <tableColumn id="5" name="Level" dataDxfId="32"/>
+    <tableColumn id="6" name="Rare" dataDxfId="31"/>
+    <tableColumn id="7" name="MaxPile" dataDxfId="30"/>
+    <tableColumn id="8" name="ValueFactor" dataDxfId="29"/>
+    <tableColumn id="9" name="SubType" dataDxfId="28"/>
+    <tableColumn id="11" name="IsUsable" dataDxfId="27"/>
+    <tableColumn id="12" name="IsThrowable" dataDxfId="26"/>
+    <tableColumn id="15" name="RandomGroup" dataDxfId="25"/>
+    <tableColumn id="13" name="CdGroup" dataDxfId="24"/>
+    <tableColumn id="14" name="Url" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表1_34" displayName="表1_34" ref="A3:N97" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27" tableBorderDxfId="26">
-  <autoFilter ref="A3:N97"/>
-  <sortState ref="A4:N96">
-    <sortCondition ref="A3:A96"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表1_34" displayName="表1_34" ref="A3:N98" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21" tableBorderDxfId="20">
+  <autoFilter ref="A3:N98"/>
+  <sortState ref="A4:N97">
+    <sortCondition ref="A3:A97"/>
   </sortState>
   <tableColumns count="14">
-    <tableColumn id="1" name="Id" dataDxfId="25"/>
-    <tableColumn id="2" name="Name" dataDxfId="24"/>
-    <tableColumn id="3" name="Type" dataDxfId="23"/>
-    <tableColumn id="4" name="Descript" dataDxfId="22"/>
-    <tableColumn id="5" name="Level" dataDxfId="21"/>
-    <tableColumn id="6" name="Rare" dataDxfId="20"/>
-    <tableColumn id="7" name="MaxPile" dataDxfId="19"/>
-    <tableColumn id="8" name="ValueFactor" dataDxfId="18"/>
-    <tableColumn id="9" name="SubType" dataDxfId="17"/>
-    <tableColumn id="11" name="IsUsable" dataDxfId="16"/>
-    <tableColumn id="12" name="IsThrowable" dataDxfId="15"/>
-    <tableColumn id="15" name="RandomGroup" dataDxfId="14"/>
-    <tableColumn id="13" name="CdGroup" dataDxfId="13"/>
-    <tableColumn id="14" name="Url" dataDxfId="12"/>
+    <tableColumn id="1" name="Id" dataDxfId="19"/>
+    <tableColumn id="2" name="Name" dataDxfId="18"/>
+    <tableColumn id="3" name="Type" dataDxfId="17"/>
+    <tableColumn id="4" name="Descript" dataDxfId="16"/>
+    <tableColumn id="5" name="Level" dataDxfId="15"/>
+    <tableColumn id="6" name="Rare" dataDxfId="14"/>
+    <tableColumn id="7" name="MaxPile" dataDxfId="13"/>
+    <tableColumn id="8" name="ValueFactor" dataDxfId="12"/>
+    <tableColumn id="9" name="SubType" dataDxfId="11"/>
+    <tableColumn id="11" name="IsUsable" dataDxfId="10"/>
+    <tableColumn id="12" name="IsThrowable" dataDxfId="9"/>
+    <tableColumn id="15" name="RandomGroup" dataDxfId="8"/>
+    <tableColumn id="13" name="CdGroup" dataDxfId="7"/>
+    <tableColumn id="14" name="Url" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="CAEACD"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -7102,6 +7004,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -7137,6 +7056,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -21601,7 +21537,7 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="A4:N347">
-    <cfRule type="containsBlanks" dxfId="11" priority="1">
+    <cfRule type="containsBlanks" dxfId="5" priority="1">
       <formula>LEN(TRIM(A4))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22332,12 +22268,12 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="A4:N20">
-    <cfRule type="containsBlanks" dxfId="10" priority="2">
+    <cfRule type="containsBlanks" dxfId="4" priority="2">
       <formula>LEN(TRIM(A4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:N20">
-    <cfRule type="containsBlanks" dxfId="9" priority="1">
+    <cfRule type="containsBlanks" dxfId="3" priority="1">
       <formula>LEN(TRIM(A15))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22352,13 +22288,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N97"/>
+  <dimension ref="A1:N98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B61" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F87" sqref="F87"/>
+      <selection pane="bottomRight" activeCell="D73" sqref="D73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -25159,22 +25095,22 @@
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A73">
-        <v>22033030</v>
+        <v>22033019</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>1233</v>
+        <v>1385</v>
       </c>
       <c r="C73" s="7">
         <v>1</v>
       </c>
       <c r="D73" t="s">
-        <v>1227</v>
+        <v>1386</v>
       </c>
       <c r="E73">
         <v>1</v>
       </c>
       <c r="F73">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G73">
         <v>99</v>
@@ -25183,7 +25119,7 @@
         <v>200</v>
       </c>
       <c r="I73">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="J73" t="s">
         <v>1032</v>
@@ -25191,31 +25127,28 @@
       <c r="K73" t="s">
         <v>1032</v>
       </c>
-      <c r="M73">
-        <v>1</v>
-      </c>
       <c r="N73" t="s">
-        <v>1230</v>
+        <v>1384</v>
       </c>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A74">
-        <v>22033031</v>
+        <v>22033030</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="C74" s="7">
         <v>1</v>
       </c>
       <c r="D74" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="E74">
         <v>1</v>
       </c>
       <c r="F74">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G74">
         <v>99</v>
@@ -25236,27 +25169,27 @@
         <v>1</v>
       </c>
       <c r="N74" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A75">
-        <v>22033032</v>
+        <v>22033031</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="C75" s="7">
         <v>1</v>
       </c>
       <c r="D75" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="E75">
         <v>1</v>
       </c>
       <c r="F75">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G75">
         <v>99</v>
@@ -25277,27 +25210,27 @@
         <v>1</v>
       </c>
       <c r="N75" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A76">
-        <v>22034001</v>
+        <v>22033032</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>962</v>
+        <v>1235</v>
       </c>
       <c r="C76" s="7">
         <v>1</v>
       </c>
       <c r="D76" t="s">
-        <v>1195</v>
+        <v>1229</v>
       </c>
       <c r="E76">
         <v>1</v>
       </c>
       <c r="F76">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G76">
         <v>99</v>
@@ -25306,36 +25239,39 @@
         <v>200</v>
       </c>
       <c r="I76">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J76" t="s">
-        <v>1039</v>
+        <v>1032</v>
       </c>
       <c r="K76" t="s">
         <v>1032</v>
       </c>
+      <c r="M76">
+        <v>1</v>
+      </c>
       <c r="N76" t="s">
-        <v>963</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A77">
-        <v>22034002</v>
+        <v>22034001</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>964</v>
+        <v>962</v>
       </c>
       <c r="C77" s="7">
         <v>1</v>
       </c>
       <c r="D77" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="E77">
         <v>1</v>
       </c>
       <c r="F77">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G77">
         <v>99</v>
@@ -25347,33 +25283,33 @@
         <v>13</v>
       </c>
       <c r="J77" t="s">
-        <v>1032</v>
+        <v>1039</v>
       </c>
       <c r="K77" t="s">
         <v>1032</v>
       </c>
       <c r="N77" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A78">
-        <v>22034003</v>
+        <v>22034002</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>1198</v>
+        <v>964</v>
       </c>
       <c r="C78" s="7">
         <v>1</v>
       </c>
       <c r="D78" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="E78">
         <v>1</v>
       </c>
       <c r="F78">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G78">
         <v>99</v>
@@ -25382,7 +25318,7 @@
         <v>200</v>
       </c>
       <c r="I78">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="J78" t="s">
         <v>1032</v>
@@ -25390,25 +25326,22 @@
       <c r="K78" t="s">
         <v>1032</v>
       </c>
-      <c r="M78">
-        <v>4</v>
-      </c>
       <c r="N78" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A79">
-        <v>22034004</v>
+        <v>22034003</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>967</v>
+        <v>1198</v>
       </c>
       <c r="C79" s="7">
         <v>1</v>
       </c>
       <c r="D79" t="s">
-        <v>1221</v>
+        <v>1197</v>
       </c>
       <c r="E79">
         <v>1</v>
@@ -25435,21 +25368,21 @@
         <v>4</v>
       </c>
       <c r="N79" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A80">
-        <v>22034005</v>
+        <v>22034004</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
       <c r="C80" s="7">
         <v>1</v>
       </c>
       <c r="D80" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="E80">
         <v>1</v>
@@ -25476,21 +25409,21 @@
         <v>4</v>
       </c>
       <c r="N80" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A81">
-        <v>22034006</v>
+        <v>22034005</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
       <c r="C81" s="7">
         <v>1</v>
       </c>
       <c r="D81" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="E81">
         <v>1</v>
@@ -25517,21 +25450,21 @@
         <v>4</v>
       </c>
       <c r="N81" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A82">
-        <v>22034007</v>
+        <v>22034006</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
       <c r="C82" s="7">
         <v>1</v>
       </c>
       <c r="D82" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="E82">
         <v>1</v>
@@ -25558,21 +25491,21 @@
         <v>4</v>
       </c>
       <c r="N82" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A83">
-        <v>22034008</v>
+        <v>22034007</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
       <c r="C83" s="7">
         <v>1</v>
       </c>
       <c r="D83" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="E83">
         <v>1</v>
@@ -25599,21 +25532,21 @@
         <v>4</v>
       </c>
       <c r="N83" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A84">
-        <v>22034009</v>
+        <v>22034008</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>1199</v>
+        <v>975</v>
       </c>
       <c r="C84" s="7">
         <v>1</v>
       </c>
       <c r="D84" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="E84">
         <v>1</v>
@@ -25640,21 +25573,21 @@
         <v>4</v>
       </c>
       <c r="N84" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A85">
-        <v>22034010</v>
+        <v>22034009</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>1381</v>
+        <v>1199</v>
       </c>
       <c r="C85" s="7">
         <v>1</v>
       </c>
       <c r="D85" t="s">
-        <v>1375</v>
+        <v>1226</v>
       </c>
       <c r="E85">
         <v>1</v>
@@ -25669,7 +25602,7 @@
         <v>200</v>
       </c>
       <c r="I85">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J85" t="s">
         <v>1032</v>
@@ -25681,21 +25614,21 @@
         <v>4</v>
       </c>
       <c r="N85" t="s">
-        <v>1378</v>
+        <v>977</v>
       </c>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A86">
-        <v>22034011</v>
+        <v>22034010</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="C86" s="7">
         <v>1</v>
       </c>
       <c r="D86" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
       <c r="E86">
         <v>1</v>
@@ -25718,22 +25651,25 @@
       <c r="K86" t="s">
         <v>1032</v>
       </c>
+      <c r="M86">
+        <v>4</v>
+      </c>
       <c r="N86" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A87">
-        <v>22034012</v>
+        <v>22034011</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="C87" s="7">
         <v>1</v>
       </c>
       <c r="D87" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="E87">
         <v>1</v>
@@ -25757,27 +25693,27 @@
         <v>1032</v>
       </c>
       <c r="N87" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A88">
-        <v>22035001</v>
+        <v>22034012</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>978</v>
+        <v>1383</v>
       </c>
       <c r="C88" s="7">
         <v>1</v>
       </c>
       <c r="D88" t="s">
-        <v>1178</v>
+        <v>1377</v>
       </c>
       <c r="E88">
         <v>1</v>
       </c>
       <c r="F88">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G88">
         <v>99</v>
@@ -25786,24 +25722,24 @@
         <v>200</v>
       </c>
       <c r="I88">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J88" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="K88" t="s">
         <v>1032</v>
       </c>
       <c r="N88" t="s">
-        <v>979</v>
+        <v>1380</v>
       </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A89">
-        <v>22035002</v>
+        <v>22035001</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
       <c r="C89" s="7">
         <v>1</v>
@@ -25815,7 +25751,7 @@
         <v>1</v>
       </c>
       <c r="F89">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G89">
         <v>99</v>
@@ -25827,21 +25763,21 @@
         <v>16</v>
       </c>
       <c r="J89" t="s">
-        <v>1032</v>
+        <v>1033</v>
       </c>
       <c r="K89" t="s">
         <v>1032</v>
       </c>
       <c r="N89" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A90">
-        <v>22035003</v>
+        <v>22035002</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
       <c r="C90" s="7">
         <v>1</v>
@@ -25853,7 +25789,7 @@
         <v>1</v>
       </c>
       <c r="F90">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G90">
         <v>99</v>
@@ -25871,33 +25807,36 @@
         <v>1032</v>
       </c>
       <c r="N90" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A91">
-        <v>22037001</v>
+        <v>22035003</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
       <c r="C91" s="7">
         <v>1</v>
       </c>
       <c r="D91" t="s">
-        <v>985</v>
+        <v>1178</v>
       </c>
       <c r="E91">
         <v>1</v>
       </c>
+      <c r="F91">
+        <v>6</v>
+      </c>
       <c r="G91">
         <v>99</v>
       </c>
       <c r="H91">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="I91">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J91" t="s">
         <v>1032</v>
@@ -25906,21 +25845,21 @@
         <v>1032</v>
       </c>
       <c r="N91" t="s">
-        <v>986</v>
+        <v>983</v>
       </c>
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A92">
-        <v>22037002</v>
+        <v>22037001</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>1240</v>
+        <v>984</v>
       </c>
       <c r="C92" s="7">
         <v>1</v>
       </c>
       <c r="D92" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="E92">
         <v>1</v>
@@ -25941,21 +25880,21 @@
         <v>1032</v>
       </c>
       <c r="N92" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A93">
-        <v>22037003</v>
+        <v>22037002</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>989</v>
+        <v>1240</v>
       </c>
       <c r="C93" s="7">
         <v>1</v>
       </c>
       <c r="D93" t="s">
-        <v>990</v>
+        <v>987</v>
       </c>
       <c r="E93">
         <v>1</v>
@@ -25976,21 +25915,21 @@
         <v>1032</v>
       </c>
       <c r="N93" t="s">
-        <v>991</v>
+        <v>988</v>
       </c>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A94">
-        <v>22037004</v>
+        <v>22037003</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>992</v>
+        <v>989</v>
       </c>
       <c r="C94" s="7">
         <v>1</v>
       </c>
       <c r="D94" t="s">
-        <v>993</v>
+        <v>990</v>
       </c>
       <c r="E94">
         <v>1</v>
@@ -26011,21 +25950,21 @@
         <v>1032</v>
       </c>
       <c r="N94" t="s">
-        <v>994</v>
+        <v>991</v>
       </c>
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A95">
-        <v>22037101</v>
+        <v>22037004</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>995</v>
+        <v>992</v>
       </c>
       <c r="C95" s="7">
         <v>1</v>
       </c>
       <c r="D95" t="s">
-        <v>996</v>
+        <v>993</v>
       </c>
       <c r="E95">
         <v>1</v>
@@ -26037,30 +25976,30 @@
         <v>50</v>
       </c>
       <c r="I95">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="J95" t="s">
-        <v>1039</v>
+        <v>1032</v>
       </c>
       <c r="K95" t="s">
         <v>1032</v>
       </c>
       <c r="N95" t="s">
-        <v>997</v>
+        <v>994</v>
       </c>
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A96">
-        <v>22037102</v>
+        <v>22037101</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>1241</v>
+        <v>995</v>
       </c>
       <c r="C96" s="7">
         <v>1</v>
       </c>
       <c r="D96" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="E96">
         <v>1</v>
@@ -26075,27 +26014,27 @@
         <v>13</v>
       </c>
       <c r="J96" t="s">
-        <v>1032</v>
+        <v>1039</v>
       </c>
       <c r="K96" t="s">
         <v>1032</v>
       </c>
       <c r="N96" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
     </row>
     <row r="97" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A97">
-        <v>22037103</v>
+        <v>22037102</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>1000</v>
+        <v>1241</v>
       </c>
       <c r="C97" s="7">
         <v>1</v>
       </c>
       <c r="D97" t="s">
-        <v>1236</v>
+        <v>998</v>
       </c>
       <c r="E97">
         <v>1</v>
@@ -26107,36 +26046,71 @@
         <v>50</v>
       </c>
       <c r="I97">
+        <v>13</v>
+      </c>
+      <c r="J97" t="s">
+        <v>1032</v>
+      </c>
+      <c r="K97" t="s">
+        <v>1032</v>
+      </c>
+      <c r="N97" t="s">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="98" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A98">
+        <v>22037103</v>
+      </c>
+      <c r="B98" s="7" t="s">
+        <v>1000</v>
+      </c>
+      <c r="C98" s="7">
+        <v>1</v>
+      </c>
+      <c r="D98" t="s">
+        <v>1236</v>
+      </c>
+      <c r="E98">
+        <v>1</v>
+      </c>
+      <c r="G98">
+        <v>99</v>
+      </c>
+      <c r="H98">
+        <v>50</v>
+      </c>
+      <c r="I98">
         <v>11</v>
       </c>
-      <c r="J97" t="s">
-        <v>1032</v>
-      </c>
-      <c r="K97" t="s">
-        <v>1032</v>
-      </c>
-      <c r="M97">
-        <v>1</v>
-      </c>
-      <c r="N97" t="s">
+      <c r="J98" t="s">
+        <v>1032</v>
+      </c>
+      <c r="K98" t="s">
+        <v>1032</v>
+      </c>
+      <c r="M98">
+        <v>1</v>
+      </c>
+      <c r="N98" t="s">
         <v>1001</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="D4:N7 D8:K11 M8:N11 L8:L86 M15:N86 D15:K84 H5:H86 D88:N97 J87:N87 J85:K86 D85:H87">
-    <cfRule type="containsBlanks" dxfId="8" priority="3">
+  <conditionalFormatting sqref="D4:N7 D8:K11 M8:N11 D89:N98 J88:N88 J86:K87 D86:H88 L8:L72 M15:N72 D15:K72 H5:H72 D74:K85 H74:H87 L74:N87 D73:N73">
+    <cfRule type="containsBlanks" dxfId="2" priority="3">
       <formula>LEN(TRIM(D4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12:K14 M12:N14">
-    <cfRule type="containsBlanks" dxfId="7" priority="2">
+    <cfRule type="containsBlanks" dxfId="1" priority="2">
       <formula>LEN(TRIM(D12))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I85:I87">
-    <cfRule type="containsBlanks" dxfId="5" priority="1">
-      <formula>LEN(TRIM(I85))=0</formula>
+  <conditionalFormatting sqref="I86:I88">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(I86))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix the card cd group visual bug
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/HItem.xlsx
+++ b/ConfigData/Xlsx/HItem.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="材料" sheetId="1" r:id="rId1"/>
@@ -6571,69 +6571,6 @@
   </cellStyles>
   <dxfs count="59">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -7075,6 +7012,55 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -7504,6 +7490,13 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -7913,6 +7906,13 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -7927,78 +7927,78 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:N347" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57" tableBorderDxfId="56">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:N347" totalsRowShown="0" headerRowDxfId="57" dataDxfId="56" tableBorderDxfId="55">
   <autoFilter ref="A3:N347"/>
   <sortState ref="A4:N347">
     <sortCondition ref="A3:A347"/>
   </sortState>
   <tableColumns count="14">
-    <tableColumn id="1" name="Id" dataDxfId="55"/>
-    <tableColumn id="2" name="Name" dataDxfId="54"/>
+    <tableColumn id="1" name="Id" dataDxfId="54"/>
+    <tableColumn id="2" name="Name" dataDxfId="53"/>
     <tableColumn id="10" name="Ename"/>
-    <tableColumn id="3" name="Type" dataDxfId="53"/>
-    <tableColumn id="4" name="Descript" dataDxfId="52"/>
-    <tableColumn id="5" name="Level" dataDxfId="51"/>
-    <tableColumn id="6" name="Rare" dataDxfId="50"/>
-    <tableColumn id="7" name="MaxPile" dataDxfId="49"/>
-    <tableColumn id="8" name="ValueFactor" dataDxfId="48"/>
-    <tableColumn id="9" name="SubType" dataDxfId="47"/>
-    <tableColumn id="11" name="IsUsable" dataDxfId="46"/>
-    <tableColumn id="12" name="IsThrowable" dataDxfId="45"/>
-    <tableColumn id="15" name="RandomGroup" dataDxfId="44"/>
-    <tableColumn id="14" name="Url" dataDxfId="43"/>
+    <tableColumn id="3" name="Type" dataDxfId="52"/>
+    <tableColumn id="4" name="Descript" dataDxfId="51"/>
+    <tableColumn id="5" name="Level" dataDxfId="50"/>
+    <tableColumn id="6" name="Rare" dataDxfId="49"/>
+    <tableColumn id="7" name="MaxPile" dataDxfId="48"/>
+    <tableColumn id="8" name="ValueFactor" dataDxfId="47"/>
+    <tableColumn id="9" name="SubType" dataDxfId="46"/>
+    <tableColumn id="11" name="IsUsable" dataDxfId="45"/>
+    <tableColumn id="12" name="IsThrowable" dataDxfId="44"/>
+    <tableColumn id="15" name="RandomGroup" dataDxfId="43"/>
+    <tableColumn id="14" name="Url" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A3:N20" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41" tableBorderDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A3:N20" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39" tableBorderDxfId="38">
   <autoFilter ref="A3:N20"/>
   <sortState ref="A4:O435">
     <sortCondition ref="A3:A435"/>
   </sortState>
   <tableColumns count="14">
-    <tableColumn id="1" name="Id" dataDxfId="39"/>
-    <tableColumn id="2" name="Name" dataDxfId="38"/>
-    <tableColumn id="10" name="Ename" dataDxfId="37"/>
-    <tableColumn id="3" name="Type" dataDxfId="36"/>
-    <tableColumn id="4" name="Descript" dataDxfId="35"/>
-    <tableColumn id="5" name="Level" dataDxfId="34"/>
-    <tableColumn id="6" name="Rare" dataDxfId="33"/>
-    <tableColumn id="7" name="MaxPile" dataDxfId="32"/>
-    <tableColumn id="8" name="ValueFactor" dataDxfId="31"/>
-    <tableColumn id="9" name="SubType" dataDxfId="30"/>
-    <tableColumn id="11" name="IsUsable" dataDxfId="29"/>
-    <tableColumn id="12" name="IsThrowable" dataDxfId="28"/>
-    <tableColumn id="15" name="RandomGroup" dataDxfId="27"/>
-    <tableColumn id="14" name="Url" dataDxfId="26"/>
+    <tableColumn id="1" name="Id" dataDxfId="37"/>
+    <tableColumn id="2" name="Name" dataDxfId="36"/>
+    <tableColumn id="10" name="Ename" dataDxfId="35"/>
+    <tableColumn id="3" name="Type" dataDxfId="34"/>
+    <tableColumn id="4" name="Descript" dataDxfId="33"/>
+    <tableColumn id="5" name="Level" dataDxfId="32"/>
+    <tableColumn id="6" name="Rare" dataDxfId="31"/>
+    <tableColumn id="7" name="MaxPile" dataDxfId="30"/>
+    <tableColumn id="8" name="ValueFactor" dataDxfId="29"/>
+    <tableColumn id="9" name="SubType" dataDxfId="28"/>
+    <tableColumn id="11" name="IsUsable" dataDxfId="27"/>
+    <tableColumn id="12" name="IsThrowable" dataDxfId="26"/>
+    <tableColumn id="15" name="RandomGroup" dataDxfId="25"/>
+    <tableColumn id="14" name="Url" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表1_34" displayName="表1_34" ref="A3:N114" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24" tableBorderDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表1_34" displayName="表1_34" ref="A3:N114" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15" tableBorderDxfId="14">
   <autoFilter ref="A3:N114"/>
   <sortState ref="A4:N114">
     <sortCondition ref="A3:A114"/>
   </sortState>
   <tableColumns count="14">
-    <tableColumn id="1" name="Id" dataDxfId="22"/>
-    <tableColumn id="2" name="Name" dataDxfId="21"/>
-    <tableColumn id="10" name="Ename" dataDxfId="20"/>
-    <tableColumn id="3" name="Type" dataDxfId="19"/>
-    <tableColumn id="4" name="Descript" dataDxfId="18"/>
-    <tableColumn id="5" name="Level" dataDxfId="17"/>
-    <tableColumn id="6" name="Rare" dataDxfId="16"/>
-    <tableColumn id="7" name="MaxPile" dataDxfId="15"/>
-    <tableColumn id="8" name="ValueFactor" dataDxfId="14"/>
-    <tableColumn id="9" name="SubType" dataDxfId="13"/>
-    <tableColumn id="11" name="IsUsable" dataDxfId="12"/>
-    <tableColumn id="12" name="IsThrowable" dataDxfId="11"/>
-    <tableColumn id="15" name="RandomGroup" dataDxfId="10"/>
-    <tableColumn id="14" name="Url" dataDxfId="9"/>
+    <tableColumn id="1" name="Id" dataDxfId="13"/>
+    <tableColumn id="2" name="Name" dataDxfId="12"/>
+    <tableColumn id="10" name="Ename" dataDxfId="11"/>
+    <tableColumn id="3" name="Type" dataDxfId="10"/>
+    <tableColumn id="4" name="Descript" dataDxfId="9"/>
+    <tableColumn id="5" name="Level" dataDxfId="8"/>
+    <tableColumn id="6" name="Rare" dataDxfId="7"/>
+    <tableColumn id="7" name="MaxPile" dataDxfId="6"/>
+    <tableColumn id="8" name="ValueFactor" dataDxfId="5"/>
+    <tableColumn id="9" name="SubType" dataDxfId="4"/>
+    <tableColumn id="11" name="IsUsable" dataDxfId="3"/>
+    <tableColumn id="12" name="IsThrowable" dataDxfId="2"/>
+    <tableColumn id="15" name="RandomGroup" dataDxfId="1"/>
+    <tableColumn id="14" name="Url" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8327,7 +8327,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N347"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
@@ -23616,7 +23616,7 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="A4:N347">
-    <cfRule type="containsBlanks" dxfId="8" priority="1">
+    <cfRule type="containsBlanks" dxfId="58" priority="1">
       <formula>LEN(TRIM(A4))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23633,11 +23633,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="N1" sqref="N1:N1048576"/>
+      <selection pane="bottomRight" activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -23805,10 +23805,10 @@
         <v>1</v>
       </c>
       <c r="J4">
-        <v>3</v>
-      </c>
-      <c r="K4" t="s">
-        <v>1020</v>
+        <v>16</v>
+      </c>
+      <c r="K4" s="18" t="s">
+        <v>1018</v>
       </c>
       <c r="L4" t="s">
         <v>1020</v>
@@ -24392,7 +24392,7 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="A4:N20">
-    <cfRule type="containsBlanks" dxfId="7" priority="2">
+    <cfRule type="containsBlanks" dxfId="41" priority="2">
       <formula>LEN(TRIM(A4))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -24410,7 +24410,7 @@
   <dimension ref="A1:N114"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B88" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="N1" sqref="N1:N1048576"/>
@@ -29070,37 +29070,37 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="E8:L8 K102:L103 E90:L101 I90:I106 E102:I107 E9:I11 K9:L11 I5:I21 M8:M21 E15:L21 E4:M7 M90:M103 K104:M107 E108:M114 E38:M89 N4:N114">
-    <cfRule type="containsBlanks" dxfId="6" priority="7">
+    <cfRule type="containsBlanks" dxfId="23" priority="7">
       <formula>LEN(TRIM(E4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12:L14">
-    <cfRule type="containsBlanks" dxfId="5" priority="6">
+    <cfRule type="containsBlanks" dxfId="22" priority="6">
       <formula>LEN(TRIM(E12))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J102:J104">
-    <cfRule type="containsBlanks" dxfId="4" priority="5">
+    <cfRule type="containsBlanks" dxfId="21" priority="5">
       <formula>LEN(TRIM(J102))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J105:J107">
-    <cfRule type="containsBlanks" dxfId="3" priority="4">
+    <cfRule type="containsBlanks" dxfId="20" priority="4">
       <formula>LEN(TRIM(J105))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9:J11">
-    <cfRule type="containsBlanks" dxfId="2" priority="3">
+    <cfRule type="containsBlanks" dxfId="19" priority="3">
       <formula>LEN(TRIM(J9))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I22:I37 M22:M37">
-    <cfRule type="containsBlanks" dxfId="1" priority="2">
+    <cfRule type="containsBlanks" dxfId="18" priority="2">
       <formula>LEN(TRIM(I22))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22:L37">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
+    <cfRule type="containsBlanks" dxfId="17" priority="1">
       <formula>LEN(TRIM(E22))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
fix some quest bugs
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/HItem.xlsx
+++ b/ConfigData/Xlsx/HItem.xlsx
@@ -6532,100 +6532,6 @@
   </cellStyles>
   <dxfs count="57">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -6885,6 +6791,25 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
@@ -7036,6 +6961,41 @@
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="3" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -7299,6 +7259,25 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
@@ -7438,6 +7417,20 @@
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="3" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -7824,6 +7817,13 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -7838,78 +7838,78 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:N347" totalsRowShown="0" headerRowDxfId="56" dataDxfId="55" tableBorderDxfId="54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:N347" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54" tableBorderDxfId="53">
   <autoFilter ref="A3:N347"/>
   <sortState ref="A4:N347">
     <sortCondition ref="A3:A347"/>
   </sortState>
   <tableColumns count="14">
-    <tableColumn id="1" name="Id" dataDxfId="53"/>
-    <tableColumn id="2" name="Name" dataDxfId="52"/>
+    <tableColumn id="1" name="Id" dataDxfId="52"/>
+    <tableColumn id="2" name="Name" dataDxfId="51"/>
     <tableColumn id="10" name="Ename"/>
-    <tableColumn id="3" name="Type" dataDxfId="51"/>
+    <tableColumn id="3" name="Type" dataDxfId="50"/>
     <tableColumn id="13" name="SubType"/>
-    <tableColumn id="4" name="Descript" dataDxfId="50"/>
-    <tableColumn id="5" name="Level" dataDxfId="49"/>
-    <tableColumn id="6" name="Rare" dataDxfId="48"/>
-    <tableColumn id="7" name="MaxPile" dataDxfId="47"/>
-    <tableColumn id="8" name="ValueFactor" dataDxfId="46"/>
-    <tableColumn id="11" name="IsUsable" dataDxfId="45"/>
-    <tableColumn id="12" name="IsThrowable" dataDxfId="44"/>
-    <tableColumn id="15" name="RandomGroup" dataDxfId="43"/>
-    <tableColumn id="14" name="Url" dataDxfId="42"/>
+    <tableColumn id="4" name="Descript" dataDxfId="49"/>
+    <tableColumn id="5" name="Level" dataDxfId="48"/>
+    <tableColumn id="6" name="Rare" dataDxfId="47"/>
+    <tableColumn id="7" name="MaxPile" dataDxfId="46"/>
+    <tableColumn id="8" name="ValueFactor" dataDxfId="45"/>
+    <tableColumn id="11" name="IsUsable" dataDxfId="44"/>
+    <tableColumn id="12" name="IsThrowable" dataDxfId="43"/>
+    <tableColumn id="15" name="RandomGroup" dataDxfId="42"/>
+    <tableColumn id="14" name="Url" dataDxfId="41"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A3:N20" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40" tableBorderDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A3:N20" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37" tableBorderDxfId="36">
   <autoFilter ref="A3:N20"/>
   <sortState ref="A4:O435">
     <sortCondition ref="A3:A435"/>
   </sortState>
   <tableColumns count="14">
-    <tableColumn id="1" name="Id" dataDxfId="38"/>
-    <tableColumn id="2" name="Name" dataDxfId="37"/>
-    <tableColumn id="10" name="Ename" dataDxfId="36"/>
-    <tableColumn id="3" name="Type" dataDxfId="35"/>
-    <tableColumn id="13" name="SubType" dataDxfId="8"/>
-    <tableColumn id="4" name="Descript" dataDxfId="34"/>
-    <tableColumn id="5" name="Level" dataDxfId="33"/>
-    <tableColumn id="6" name="Rare" dataDxfId="32"/>
-    <tableColumn id="7" name="MaxPile" dataDxfId="31"/>
-    <tableColumn id="8" name="ValueFactor" dataDxfId="30"/>
-    <tableColumn id="11" name="IsUsable" dataDxfId="29"/>
-    <tableColumn id="12" name="IsThrowable" dataDxfId="28"/>
-    <tableColumn id="15" name="RandomGroup" dataDxfId="27"/>
-    <tableColumn id="14" name="Url" dataDxfId="26"/>
+    <tableColumn id="1" name="Id" dataDxfId="35"/>
+    <tableColumn id="2" name="Name" dataDxfId="34"/>
+    <tableColumn id="10" name="Ename" dataDxfId="33"/>
+    <tableColumn id="3" name="Type" dataDxfId="32"/>
+    <tableColumn id="13" name="SubType" dataDxfId="31"/>
+    <tableColumn id="4" name="Descript" dataDxfId="30"/>
+    <tableColumn id="5" name="Level" dataDxfId="29"/>
+    <tableColumn id="6" name="Rare" dataDxfId="28"/>
+    <tableColumn id="7" name="MaxPile" dataDxfId="27"/>
+    <tableColumn id="8" name="ValueFactor" dataDxfId="26"/>
+    <tableColumn id="11" name="IsUsable" dataDxfId="25"/>
+    <tableColumn id="12" name="IsThrowable" dataDxfId="24"/>
+    <tableColumn id="15" name="RandomGroup" dataDxfId="23"/>
+    <tableColumn id="14" name="Url" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表1_34" displayName="表1_34" ref="A3:N115" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24" tableBorderDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表1_34" displayName="表1_34" ref="A3:N115" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15" tableBorderDxfId="14">
   <autoFilter ref="A3:N115"/>
   <sortState ref="A4:N115">
     <sortCondition ref="A3:A115"/>
   </sortState>
   <tableColumns count="14">
-    <tableColumn id="1" name="Id" dataDxfId="22"/>
-    <tableColumn id="2" name="Name" dataDxfId="21"/>
-    <tableColumn id="10" name="Ename" dataDxfId="20"/>
-    <tableColumn id="3" name="Type" dataDxfId="19"/>
+    <tableColumn id="1" name="Id" dataDxfId="13"/>
+    <tableColumn id="2" name="Name" dataDxfId="12"/>
+    <tableColumn id="10" name="Ename" dataDxfId="11"/>
+    <tableColumn id="3" name="Type" dataDxfId="10"/>
     <tableColumn id="13" name="SubType" dataDxfId="9"/>
-    <tableColumn id="4" name="Descript" dataDxfId="18"/>
-    <tableColumn id="5" name="Level" dataDxfId="17"/>
-    <tableColumn id="6" name="Rare" dataDxfId="16"/>
-    <tableColumn id="7" name="MaxPile" dataDxfId="15"/>
-    <tableColumn id="8" name="ValueFactor" dataDxfId="14"/>
-    <tableColumn id="11" name="IsUsable" dataDxfId="13"/>
-    <tableColumn id="12" name="IsThrowable" dataDxfId="12"/>
-    <tableColumn id="15" name="RandomGroup" dataDxfId="11"/>
-    <tableColumn id="14" name="Url" dataDxfId="10"/>
+    <tableColumn id="4" name="Descript" dataDxfId="8"/>
+    <tableColumn id="5" name="Level" dataDxfId="7"/>
+    <tableColumn id="6" name="Rare" dataDxfId="6"/>
+    <tableColumn id="7" name="MaxPile" dataDxfId="5"/>
+    <tableColumn id="8" name="ValueFactor" dataDxfId="4"/>
+    <tableColumn id="11" name="IsUsable" dataDxfId="3"/>
+    <tableColumn id="12" name="IsThrowable" dataDxfId="2"/>
+    <tableColumn id="15" name="RandomGroup" dataDxfId="1"/>
+    <tableColumn id="14" name="Url" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -23528,7 +23528,7 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="B4:N347">
-    <cfRule type="containsBlanks" dxfId="7" priority="1">
+    <cfRule type="containsBlanks" dxfId="56" priority="1">
       <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -24305,12 +24305,12 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="B5:N20">
-    <cfRule type="containsBlanks" dxfId="6" priority="3">
+    <cfRule type="containsBlanks" dxfId="40" priority="3">
       <formula>LEN(TRIM(B5))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:N4">
-    <cfRule type="containsBlanks" dxfId="5" priority="1">
+    <cfRule type="containsBlanks" dxfId="39" priority="1">
       <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -24328,10 +24328,10 @@
   <dimension ref="A1:N115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B65" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B62" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C74" sqref="C74"/>
+      <selection pane="bottomRight" activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -27477,7 +27477,7 @@
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A78">
-        <v>22301605</v>
+        <v>22301601</v>
       </c>
       <c r="B78" s="4" t="s">
         <v>1738</v>
@@ -27515,7 +27515,7 @@
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A79">
-        <v>22301606</v>
+        <v>22301602</v>
       </c>
       <c r="B79" s="4" t="s">
         <v>1739</v>
@@ -27553,7 +27553,7 @@
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A80">
-        <v>22301607</v>
+        <v>22301603</v>
       </c>
       <c r="B80" s="4" t="s">
         <v>1740</v>
@@ -27591,7 +27591,7 @@
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A81">
-        <v>22301608</v>
+        <v>22301604</v>
       </c>
       <c r="B81" s="4" t="s">
         <v>1741</v>
@@ -29030,27 +29030,27 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="J91:J107 F103:J108 F9:J11 J5:J21 M8:M21 E5:J8 E109:J115 K5:M7 K8:L37 E4:N4 N5:N80 K38:M80 E12:J80 E82:J102 K82:N115 E81:N81">
-    <cfRule type="containsBlanks" dxfId="4" priority="8">
+    <cfRule type="containsBlanks" dxfId="21" priority="8">
       <formula>LEN(TRIM(E4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E103:E105">
-    <cfRule type="containsBlanks" dxfId="3" priority="6">
+    <cfRule type="containsBlanks" dxfId="20" priority="6">
       <formula>LEN(TRIM(E103))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E106:E108">
-    <cfRule type="containsBlanks" dxfId="2" priority="5">
+    <cfRule type="containsBlanks" dxfId="19" priority="5">
       <formula>LEN(TRIM(E106))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9:E11">
-    <cfRule type="containsBlanks" dxfId="1" priority="4">
+    <cfRule type="containsBlanks" dxfId="18" priority="4">
       <formula>LEN(TRIM(E9))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J22:J37 M22:M37">
-    <cfRule type="containsBlanks" dxfId="0" priority="3">
+    <cfRule type="containsBlanks" dxfId="17" priority="3">
       <formula>LEN(TRIM(J22))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
add some tradable items
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/HItem.xlsx
+++ b/ConfigData/Xlsx/HItem.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" activeTab="1"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="材料" sheetId="1" r:id="rId1"/>
@@ -20,17 +20,17 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'~素材类型分析'!$A$1:$B$19</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Real</author>
   </authors>
   <commentList>
-    <comment ref="D1" authorId="0" shapeId="0">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -89,12 +89,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Real</author>
   </authors>
   <commentList>
-    <comment ref="D1" authorId="0" shapeId="0">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -153,12 +153,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Real</author>
   </authors>
   <commentList>
-    <comment ref="D1" authorId="0" shapeId="0">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -217,7 +217,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3379" uniqueCount="1964">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3463" uniqueCount="1995">
   <si>
     <t>血蓟</t>
   </si>
@@ -6684,13 +6684,137 @@
   </si>
   <si>
     <t>RandomGroup</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>盐</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>spyan</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>一种调味剂</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>spyan</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>糖</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>sptang</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>sptang</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>香料</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>spxiangliao</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>面粉</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>spmianfen</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>茶叶</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>spcha</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>咖啡</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>spkafei</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>可可</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>spkeke</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>大豆</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>玉米</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>水稻</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>spdadou</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>spyumi</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>spshuidao</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>小麦</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>spxiaomai</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>土豆</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>sptudou</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>地瓜</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>spdigua</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>南瓜</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>spnangua</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -7600,26 +7724,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
@@ -8133,6 +8237,26 @@
         <vertical/>
         <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <font>
@@ -8897,84 +9021,84 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:P355" totalsRowShown="0" headerRowDxfId="63" dataDxfId="62" tableBorderDxfId="61">
-  <autoFilter ref="A3:P355"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表1" displayName="表1" ref="A3:P369" totalsRowShown="0" headerRowDxfId="63" dataDxfId="62" tableBorderDxfId="61">
+  <autoFilter ref="A3:P369" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState ref="A4:P347">
     <sortCondition ref="A3:A347"/>
   </sortState>
   <tableColumns count="16">
-    <tableColumn id="1" name="Id" dataDxfId="60"/>
-    <tableColumn id="2" name="Name" dataDxfId="59"/>
-    <tableColumn id="10" name="Ename"/>
-    <tableColumn id="3" name="Type" dataDxfId="58"/>
-    <tableColumn id="13" name="SubType"/>
-    <tableColumn id="4" name="Descript" dataDxfId="57"/>
-    <tableColumn id="5" name="Level" dataDxfId="56"/>
-    <tableColumn id="6" name="Rare" dataDxfId="55"/>
-    <tableColumn id="7" name="MaxPile" dataDxfId="54"/>
-    <tableColumn id="8" name="ValueFactor" dataDxfId="53"/>
-    <tableColumn id="11" name="IsUsable" dataDxfId="52"/>
-    <tableColumn id="12" name="IsThrowable" dataDxfId="51"/>
-    <tableColumn id="16" name="RandomGroup"/>
-    <tableColumn id="15" name="Frequency" dataDxfId="50"/>
-    <tableColumn id="9" name="Attributes"/>
-    <tableColumn id="14" name="Url" dataDxfId="49"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="60"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="59"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Ename"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Type" dataDxfId="58"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="SubType"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Descript" dataDxfId="57"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Level" dataDxfId="56"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Rare" dataDxfId="55"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="MaxPile" dataDxfId="54"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="ValueFactor" dataDxfId="53"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="IsUsable" dataDxfId="52"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="IsThrowable" dataDxfId="51"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="RandomGroup"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Frequency" dataDxfId="50"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Attributes"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Url" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A3:P20" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47" tableBorderDxfId="46">
-  <autoFilter ref="A3:P20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="表1_3" displayName="表1_3" ref="A3:P20" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47" tableBorderDxfId="46">
+  <autoFilter ref="A3:P20" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <sortState ref="A4:Q435">
     <sortCondition ref="A3:A435"/>
   </sortState>
   <tableColumns count="16">
-    <tableColumn id="1" name="Id" dataDxfId="45"/>
-    <tableColumn id="2" name="Name" dataDxfId="44"/>
-    <tableColumn id="10" name="Ename" dataDxfId="43"/>
-    <tableColumn id="3" name="Type" dataDxfId="42"/>
-    <tableColumn id="13" name="SubType" dataDxfId="41"/>
-    <tableColumn id="4" name="Descript" dataDxfId="40"/>
-    <tableColumn id="5" name="Level" dataDxfId="39"/>
-    <tableColumn id="6" name="Rare" dataDxfId="38"/>
-    <tableColumn id="7" name="MaxPile" dataDxfId="37"/>
-    <tableColumn id="8" name="ValueFactor" dataDxfId="36"/>
-    <tableColumn id="11" name="IsUsable" dataDxfId="35"/>
-    <tableColumn id="12" name="IsThrowable" dataDxfId="34"/>
-    <tableColumn id="16" name="RandomGroup" dataDxfId="12"/>
-    <tableColumn id="15" name="Frequency" dataDxfId="33"/>
-    <tableColumn id="9" name="Attributes" dataDxfId="32"/>
-    <tableColumn id="14" name="Url" dataDxfId="31"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Id" dataDxfId="45"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Name" dataDxfId="44"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Ename" dataDxfId="43"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Type" dataDxfId="42"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="SubType" dataDxfId="41"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Descript" dataDxfId="40"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Level" dataDxfId="39"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Rare" dataDxfId="38"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="MaxPile" dataDxfId="37"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="ValueFactor" dataDxfId="36"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="IsUsable" dataDxfId="35"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="IsThrowable" dataDxfId="34"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="RandomGroup" dataDxfId="33"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="Frequency" dataDxfId="32"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Attributes" dataDxfId="31"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="Url" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表1_34" displayName="表1_34" ref="A3:P121" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29" tableBorderDxfId="28">
-  <autoFilter ref="A3:P121"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="表1_34" displayName="表1_34" ref="A3:P121" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28" tableBorderDxfId="27">
+  <autoFilter ref="A3:P121" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <sortState ref="A4:P121">
     <sortCondition ref="A3:A121"/>
   </sortState>
   <tableColumns count="16">
-    <tableColumn id="1" name="Id" dataDxfId="27"/>
-    <tableColumn id="2" name="Name" dataDxfId="26"/>
-    <tableColumn id="10" name="Ename" dataDxfId="25"/>
-    <tableColumn id="3" name="Type" dataDxfId="24"/>
-    <tableColumn id="13" name="SubType" dataDxfId="23"/>
-    <tableColumn id="4" name="Descript" dataDxfId="22"/>
-    <tableColumn id="5" name="Level" dataDxfId="21"/>
-    <tableColumn id="6" name="Rare" dataDxfId="20"/>
-    <tableColumn id="7" name="MaxPile" dataDxfId="19"/>
-    <tableColumn id="8" name="ValueFactor" dataDxfId="18"/>
-    <tableColumn id="11" name="IsUsable" dataDxfId="17"/>
-    <tableColumn id="12" name="IsThrowable" dataDxfId="16"/>
-    <tableColumn id="16" name="RandomGroup"/>
-    <tableColumn id="15" name="Frequency" dataDxfId="15"/>
-    <tableColumn id="9" name="Attributes" dataDxfId="14"/>
-    <tableColumn id="14" name="Url" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Id" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Name" dataDxfId="25"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="Ename" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Type" dataDxfId="23"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0200-00000D000000}" name="SubType" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Descript" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Level" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Rare" dataDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="MaxPile" dataDxfId="18"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="ValueFactor" dataDxfId="17"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="IsUsable" dataDxfId="16"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="IsThrowable" dataDxfId="15"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0200-000010000000}" name="RandomGroup"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0200-00000F000000}" name="Frequency" dataDxfId="14"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Attributes" dataDxfId="13"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0200-00000E000000}" name="Url" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9300,21 +9424,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P355"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:P369"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B342" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="M1" sqref="M1:M3"/>
+      <selection pane="bottomRight" activeCell="O369" sqref="O369"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5" customWidth="1"/>
-    <col min="5" max="5" width="6.5" customWidth="1"/>
+    <col min="4" max="5" width="3.25" customWidth="1"/>
     <col min="6" max="6" width="22.75" customWidth="1"/>
     <col min="7" max="9" width="4.75" customWidth="1"/>
     <col min="10" max="12" width="6.5" customWidth="1"/>
@@ -26900,9 +27023,667 @@
         <v>1931</v>
       </c>
     </row>
+    <row r="356" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A356" s="19">
+        <v>22120100</v>
+      </c>
+      <c r="B356" s="6" t="s">
+        <v>1964</v>
+      </c>
+      <c r="C356" t="s">
+        <v>1965</v>
+      </c>
+      <c r="D356" s="6">
+        <v>2</v>
+      </c>
+      <c r="E356">
+        <v>10</v>
+      </c>
+      <c r="F356" s="6" t="s">
+        <v>1966</v>
+      </c>
+      <c r="G356" s="6">
+        <v>1</v>
+      </c>
+      <c r="H356" s="6">
+        <v>1</v>
+      </c>
+      <c r="I356" s="6">
+        <v>99</v>
+      </c>
+      <c r="J356" s="6">
+        <v>100</v>
+      </c>
+      <c r="K356" t="s">
+        <v>907</v>
+      </c>
+      <c r="L356" t="s">
+        <v>905</v>
+      </c>
+      <c r="M356">
+        <v>3</v>
+      </c>
+      <c r="N356">
+        <v>100</v>
+      </c>
+      <c r="P356" s="6" t="s">
+        <v>1967</v>
+      </c>
+    </row>
+    <row r="357" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A357" s="19">
+        <v>22120101</v>
+      </c>
+      <c r="B357" s="6" t="s">
+        <v>1968</v>
+      </c>
+      <c r="C357" t="s">
+        <v>1969</v>
+      </c>
+      <c r="D357" s="6">
+        <v>2</v>
+      </c>
+      <c r="E357">
+        <v>10</v>
+      </c>
+      <c r="F357" s="6" t="s">
+        <v>1966</v>
+      </c>
+      <c r="G357" s="6">
+        <v>1</v>
+      </c>
+      <c r="H357" s="6">
+        <v>1</v>
+      </c>
+      <c r="I357" s="6">
+        <v>99</v>
+      </c>
+      <c r="J357" s="6">
+        <v>100</v>
+      </c>
+      <c r="K357" t="s">
+        <v>907</v>
+      </c>
+      <c r="L357" t="s">
+        <v>905</v>
+      </c>
+      <c r="M357">
+        <v>3</v>
+      </c>
+      <c r="N357">
+        <v>100</v>
+      </c>
+      <c r="P357" s="6" t="s">
+        <v>1970</v>
+      </c>
+    </row>
+    <row r="358" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A358" s="19">
+        <v>22120102</v>
+      </c>
+      <c r="B358" s="6" t="s">
+        <v>1971</v>
+      </c>
+      <c r="C358" t="s">
+        <v>1972</v>
+      </c>
+      <c r="D358" s="6">
+        <v>2</v>
+      </c>
+      <c r="E358">
+        <v>10</v>
+      </c>
+      <c r="F358" s="6" t="s">
+        <v>1966</v>
+      </c>
+      <c r="G358" s="6">
+        <v>1</v>
+      </c>
+      <c r="H358" s="6">
+        <v>1</v>
+      </c>
+      <c r="I358" s="6">
+        <v>99</v>
+      </c>
+      <c r="J358" s="6">
+        <v>100</v>
+      </c>
+      <c r="K358" t="s">
+        <v>907</v>
+      </c>
+      <c r="L358" t="s">
+        <v>905</v>
+      </c>
+      <c r="M358">
+        <v>3</v>
+      </c>
+      <c r="N358">
+        <v>100</v>
+      </c>
+      <c r="P358" t="s">
+        <v>1972</v>
+      </c>
+    </row>
+    <row r="359" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A359" s="19">
+        <v>22120103</v>
+      </c>
+      <c r="B359" s="6" t="s">
+        <v>1973</v>
+      </c>
+      <c r="C359" t="s">
+        <v>1974</v>
+      </c>
+      <c r="D359" s="6">
+        <v>2</v>
+      </c>
+      <c r="E359">
+        <v>10</v>
+      </c>
+      <c r="F359" s="6" t="s">
+        <v>1966</v>
+      </c>
+      <c r="G359" s="6">
+        <v>1</v>
+      </c>
+      <c r="H359" s="6">
+        <v>1</v>
+      </c>
+      <c r="I359" s="6">
+        <v>99</v>
+      </c>
+      <c r="J359" s="6">
+        <v>100</v>
+      </c>
+      <c r="K359" t="s">
+        <v>907</v>
+      </c>
+      <c r="L359" t="s">
+        <v>905</v>
+      </c>
+      <c r="M359">
+        <v>3</v>
+      </c>
+      <c r="N359">
+        <v>100</v>
+      </c>
+      <c r="P359" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="360" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A360" s="19">
+        <v>22120104</v>
+      </c>
+      <c r="B360" s="6" t="s">
+        <v>1975</v>
+      </c>
+      <c r="C360" t="s">
+        <v>1976</v>
+      </c>
+      <c r="D360" s="6">
+        <v>2</v>
+      </c>
+      <c r="E360">
+        <v>10</v>
+      </c>
+      <c r="F360" s="6" t="s">
+        <v>1966</v>
+      </c>
+      <c r="G360" s="6">
+        <v>1</v>
+      </c>
+      <c r="H360" s="6">
+        <v>5</v>
+      </c>
+      <c r="I360" s="6">
+        <v>99</v>
+      </c>
+      <c r="J360" s="6">
+        <v>100</v>
+      </c>
+      <c r="K360" t="s">
+        <v>907</v>
+      </c>
+      <c r="L360" t="s">
+        <v>905</v>
+      </c>
+      <c r="M360">
+        <v>3</v>
+      </c>
+      <c r="N360">
+        <v>100</v>
+      </c>
+      <c r="P360" t="s">
+        <v>1976</v>
+      </c>
+    </row>
+    <row r="361" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A361" s="19">
+        <v>22120105</v>
+      </c>
+      <c r="B361" s="6" t="s">
+        <v>1977</v>
+      </c>
+      <c r="C361" t="s">
+        <v>1978</v>
+      </c>
+      <c r="D361" s="6">
+        <v>2</v>
+      </c>
+      <c r="E361">
+        <v>10</v>
+      </c>
+      <c r="F361" s="6" t="s">
+        <v>1966</v>
+      </c>
+      <c r="G361" s="6">
+        <v>1</v>
+      </c>
+      <c r="H361" s="6">
+        <v>5</v>
+      </c>
+      <c r="I361" s="6">
+        <v>99</v>
+      </c>
+      <c r="J361" s="6">
+        <v>100</v>
+      </c>
+      <c r="K361" t="s">
+        <v>907</v>
+      </c>
+      <c r="L361" t="s">
+        <v>905</v>
+      </c>
+      <c r="M361">
+        <v>3</v>
+      </c>
+      <c r="N361">
+        <v>100</v>
+      </c>
+      <c r="P361" t="s">
+        <v>1978</v>
+      </c>
+    </row>
+    <row r="362" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A362" s="19">
+        <v>22120106</v>
+      </c>
+      <c r="B362" s="6" t="s">
+        <v>1979</v>
+      </c>
+      <c r="C362" t="s">
+        <v>1980</v>
+      </c>
+      <c r="D362" s="6">
+        <v>2</v>
+      </c>
+      <c r="E362">
+        <v>10</v>
+      </c>
+      <c r="F362" s="6" t="s">
+        <v>1966</v>
+      </c>
+      <c r="G362" s="6">
+        <v>1</v>
+      </c>
+      <c r="H362" s="6">
+        <v>5</v>
+      </c>
+      <c r="I362" s="6">
+        <v>99</v>
+      </c>
+      <c r="J362" s="6">
+        <v>100</v>
+      </c>
+      <c r="K362" t="s">
+        <v>907</v>
+      </c>
+      <c r="L362" t="s">
+        <v>905</v>
+      </c>
+      <c r="M362">
+        <v>3</v>
+      </c>
+      <c r="N362">
+        <v>100</v>
+      </c>
+      <c r="P362" t="s">
+        <v>1980</v>
+      </c>
+    </row>
+    <row r="363" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A363" s="19">
+        <v>22120107</v>
+      </c>
+      <c r="B363" s="6" t="s">
+        <v>1981</v>
+      </c>
+      <c r="C363" t="s">
+        <v>1984</v>
+      </c>
+      <c r="D363" s="6">
+        <v>2</v>
+      </c>
+      <c r="E363">
+        <v>10</v>
+      </c>
+      <c r="F363" s="6" t="s">
+        <v>1966</v>
+      </c>
+      <c r="G363" s="6">
+        <v>1</v>
+      </c>
+      <c r="H363" s="6">
+        <v>3</v>
+      </c>
+      <c r="I363" s="6">
+        <v>99</v>
+      </c>
+      <c r="J363" s="6">
+        <v>100</v>
+      </c>
+      <c r="K363" t="s">
+        <v>907</v>
+      </c>
+      <c r="L363" t="s">
+        <v>905</v>
+      </c>
+      <c r="M363">
+        <v>3</v>
+      </c>
+      <c r="N363">
+        <v>100</v>
+      </c>
+      <c r="P363" t="s">
+        <v>1984</v>
+      </c>
+    </row>
+    <row r="364" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A364" s="19">
+        <v>22120108</v>
+      </c>
+      <c r="B364" s="6" t="s">
+        <v>1982</v>
+      </c>
+      <c r="C364" t="s">
+        <v>1985</v>
+      </c>
+      <c r="D364" s="6">
+        <v>2</v>
+      </c>
+      <c r="E364">
+        <v>10</v>
+      </c>
+      <c r="F364" s="6" t="s">
+        <v>1966</v>
+      </c>
+      <c r="G364" s="6">
+        <v>1</v>
+      </c>
+      <c r="H364" s="6">
+        <v>3</v>
+      </c>
+      <c r="I364" s="6">
+        <v>99</v>
+      </c>
+      <c r="J364" s="6">
+        <v>100</v>
+      </c>
+      <c r="K364" t="s">
+        <v>907</v>
+      </c>
+      <c r="L364" t="s">
+        <v>905</v>
+      </c>
+      <c r="M364">
+        <v>3</v>
+      </c>
+      <c r="N364">
+        <v>100</v>
+      </c>
+      <c r="P364" t="s">
+        <v>1985</v>
+      </c>
+    </row>
+    <row r="365" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A365" s="19">
+        <v>22120109</v>
+      </c>
+      <c r="B365" s="6" t="s">
+        <v>1983</v>
+      </c>
+      <c r="C365" t="s">
+        <v>1986</v>
+      </c>
+      <c r="D365" s="6">
+        <v>2</v>
+      </c>
+      <c r="E365">
+        <v>10</v>
+      </c>
+      <c r="F365" s="6" t="s">
+        <v>1966</v>
+      </c>
+      <c r="G365" s="6">
+        <v>1</v>
+      </c>
+      <c r="H365" s="6">
+        <v>3</v>
+      </c>
+      <c r="I365" s="6">
+        <v>99</v>
+      </c>
+      <c r="J365" s="6">
+        <v>100</v>
+      </c>
+      <c r="K365" t="s">
+        <v>907</v>
+      </c>
+      <c r="L365" t="s">
+        <v>905</v>
+      </c>
+      <c r="M365">
+        <v>3</v>
+      </c>
+      <c r="N365">
+        <v>100</v>
+      </c>
+      <c r="P365" t="s">
+        <v>1986</v>
+      </c>
+    </row>
+    <row r="366" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A366" s="19">
+        <v>22120110</v>
+      </c>
+      <c r="B366" s="6" t="s">
+        <v>1987</v>
+      </c>
+      <c r="C366" t="s">
+        <v>1988</v>
+      </c>
+      <c r="D366" s="6">
+        <v>2</v>
+      </c>
+      <c r="E366">
+        <v>10</v>
+      </c>
+      <c r="F366" s="6" t="s">
+        <v>1966</v>
+      </c>
+      <c r="G366" s="6">
+        <v>1</v>
+      </c>
+      <c r="H366" s="6">
+        <v>3</v>
+      </c>
+      <c r="I366" s="6">
+        <v>99</v>
+      </c>
+      <c r="J366" s="6">
+        <v>100</v>
+      </c>
+      <c r="K366" t="s">
+        <v>907</v>
+      </c>
+      <c r="L366" t="s">
+        <v>905</v>
+      </c>
+      <c r="M366">
+        <v>3</v>
+      </c>
+      <c r="N366">
+        <v>100</v>
+      </c>
+      <c r="P366" t="s">
+        <v>1988</v>
+      </c>
+    </row>
+    <row r="367" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A367" s="19">
+        <v>22120111</v>
+      </c>
+      <c r="B367" s="6" t="s">
+        <v>1989</v>
+      </c>
+      <c r="C367" t="s">
+        <v>1990</v>
+      </c>
+      <c r="D367" s="6">
+        <v>2</v>
+      </c>
+      <c r="E367">
+        <v>10</v>
+      </c>
+      <c r="F367" s="6" t="s">
+        <v>1966</v>
+      </c>
+      <c r="G367" s="6">
+        <v>1</v>
+      </c>
+      <c r="H367" s="6">
+        <v>2</v>
+      </c>
+      <c r="I367" s="6">
+        <v>99</v>
+      </c>
+      <c r="J367" s="6">
+        <v>100</v>
+      </c>
+      <c r="K367" t="s">
+        <v>907</v>
+      </c>
+      <c r="L367" t="s">
+        <v>905</v>
+      </c>
+      <c r="M367">
+        <v>3</v>
+      </c>
+      <c r="N367">
+        <v>100</v>
+      </c>
+      <c r="P367" t="s">
+        <v>1990</v>
+      </c>
+    </row>
+    <row r="368" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A368" s="19">
+        <v>22120112</v>
+      </c>
+      <c r="B368" s="6" t="s">
+        <v>1991</v>
+      </c>
+      <c r="C368" t="s">
+        <v>1992</v>
+      </c>
+      <c r="D368" s="6">
+        <v>2</v>
+      </c>
+      <c r="E368">
+        <v>10</v>
+      </c>
+      <c r="F368" s="6" t="s">
+        <v>1966</v>
+      </c>
+      <c r="G368" s="6">
+        <v>1</v>
+      </c>
+      <c r="H368" s="6">
+        <v>2</v>
+      </c>
+      <c r="I368" s="6">
+        <v>99</v>
+      </c>
+      <c r="J368" s="6">
+        <v>100</v>
+      </c>
+      <c r="K368" t="s">
+        <v>907</v>
+      </c>
+      <c r="L368" t="s">
+        <v>905</v>
+      </c>
+      <c r="M368">
+        <v>3</v>
+      </c>
+      <c r="N368">
+        <v>100</v>
+      </c>
+      <c r="P368" t="s">
+        <v>1992</v>
+      </c>
+    </row>
+    <row r="369" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A369" s="19">
+        <v>22120113</v>
+      </c>
+      <c r="B369" s="6" t="s">
+        <v>1993</v>
+      </c>
+      <c r="C369" t="s">
+        <v>1994</v>
+      </c>
+      <c r="D369" s="6">
+        <v>2</v>
+      </c>
+      <c r="E369">
+        <v>10</v>
+      </c>
+      <c r="F369" s="6" t="s">
+        <v>1966</v>
+      </c>
+      <c r="G369" s="6">
+        <v>1</v>
+      </c>
+      <c r="H369" s="6">
+        <v>2</v>
+      </c>
+      <c r="I369" s="6">
+        <v>99</v>
+      </c>
+      <c r="J369" s="6">
+        <v>100</v>
+      </c>
+      <c r="K369" t="s">
+        <v>907</v>
+      </c>
+      <c r="L369" t="s">
+        <v>905</v>
+      </c>
+      <c r="M369">
+        <v>3</v>
+      </c>
+      <c r="N369">
+        <v>100</v>
+      </c>
+      <c r="P369" t="s">
+        <v>1994</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="B4:P355">
+  <conditionalFormatting sqref="B4:P369">
     <cfRule type="containsBlanks" dxfId="11" priority="1">
       <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>
@@ -26917,21 +27698,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="L3" sqref="L3"/>
+      <selection pane="bottomRight" activeCell="D1" sqref="D1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="4" max="4" width="7.25" customWidth="1"/>
-    <col min="5" max="5" width="6.5" customWidth="1"/>
+    <col min="4" max="5" width="3.25" customWidth="1"/>
     <col min="6" max="6" width="34" customWidth="1"/>
     <col min="7" max="9" width="5.75" customWidth="1"/>
     <col min="10" max="12" width="6.5" customWidth="1"/>
@@ -27746,14 +28526,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:P121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B100" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="O1" sqref="O1"/>
+      <selection pane="bottomRight" activeCell="E103" sqref="E103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -27761,8 +28541,7 @@
     <col min="1" max="1" width="10.25" customWidth="1"/>
     <col min="2" max="2" width="14.5" customWidth="1"/>
     <col min="3" max="3" width="11.125" customWidth="1"/>
-    <col min="4" max="4" width="5.5" customWidth="1"/>
-    <col min="5" max="5" width="6.5" customWidth="1"/>
+    <col min="4" max="5" width="3.75" customWidth="1"/>
     <col min="6" max="6" width="31" customWidth="1"/>
     <col min="7" max="9" width="4.875" customWidth="1"/>
     <col min="10" max="12" width="6.5" customWidth="1"/>
@@ -32743,7 +33522,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -32920,7 +33699,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B19"/>
+  <autoFilter ref="A1:B19" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add npc for lugaoyin
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/HItem.xlsx
+++ b/ConfigData/Xlsx/HItem.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18528"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -217,7 +217,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3487" uniqueCount="2020">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3493" uniqueCount="2023">
   <si>
     <t>血蓟</t>
   </si>
@@ -6908,6 +6908,17 @@
   </si>
   <si>
     <t>一种作物，能制成卷烟</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>spxiangjiaonai</t>
+  </si>
+  <si>
+    <t>香蕉牛奶</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>[特产]一种香蕉和牛奶结合而成的美味</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -7645,7 +7656,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -7737,6 +7748,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -9180,8 +9194,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表1" displayName="表1" ref="A3:P373" totalsRowShown="0" headerRowDxfId="63" dataDxfId="62" tableBorderDxfId="61">
-  <autoFilter ref="A3:P373" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表1" displayName="表1" ref="A3:P374" totalsRowShown="0" headerRowDxfId="63" dataDxfId="62" tableBorderDxfId="61">
+  <autoFilter ref="A3:P374" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState ref="A4:P347">
     <sortCondition ref="A3:A347"/>
   </sortState>
@@ -9584,10 +9598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P373"/>
+  <dimension ref="A1:P374"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B348" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B345" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="F373" sqref="F373"/>
@@ -27192,7 +27206,7 @@
       <c r="B356" s="30" t="s">
         <v>1964</v>
       </c>
-      <c r="C356" s="20" t="s">
+      <c r="C356" s="31" t="s">
         <v>1965</v>
       </c>
       <c r="D356" s="30">
@@ -27333,7 +27347,7 @@
       <c r="B359" s="30" t="s">
         <v>1993</v>
       </c>
-      <c r="C359" s="20" t="s">
+      <c r="C359" s="31" t="s">
         <v>1972</v>
       </c>
       <c r="D359" s="30">
@@ -27756,7 +27770,7 @@
       <c r="B368" s="30" t="s">
         <v>2009</v>
       </c>
-      <c r="C368" s="20" t="s">
+      <c r="C368" s="31" t="s">
         <v>1983</v>
       </c>
       <c r="D368" s="30">
@@ -27803,7 +27817,7 @@
       <c r="B369" s="30" t="s">
         <v>2011</v>
       </c>
-      <c r="C369" s="20" t="s">
+      <c r="C369" s="31" t="s">
         <v>1984</v>
       </c>
       <c r="D369" s="30">
@@ -27991,7 +28005,7 @@
       <c r="B373" s="30" t="s">
         <v>1988</v>
       </c>
-      <c r="C373" s="20" t="s">
+      <c r="C373" s="31" t="s">
         <v>1989</v>
       </c>
       <c r="D373" s="30">
@@ -28031,9 +28045,56 @@
         <v>1989</v>
       </c>
     </row>
+    <row r="374" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A374" s="29">
+        <v>22120201</v>
+      </c>
+      <c r="B374" s="6" t="s">
+        <v>2021</v>
+      </c>
+      <c r="C374" s="31" t="s">
+        <v>2020</v>
+      </c>
+      <c r="D374" s="30">
+        <v>2</v>
+      </c>
+      <c r="E374" s="20">
+        <v>10</v>
+      </c>
+      <c r="F374" s="6" t="s">
+        <v>2022</v>
+      </c>
+      <c r="G374" s="30">
+        <v>1</v>
+      </c>
+      <c r="H374" s="30">
+        <v>4</v>
+      </c>
+      <c r="I374" s="30">
+        <v>99</v>
+      </c>
+      <c r="J374" s="30">
+        <v>100</v>
+      </c>
+      <c r="K374" s="20" t="s">
+        <v>907</v>
+      </c>
+      <c r="L374" s="20" t="s">
+        <v>905</v>
+      </c>
+      <c r="M374" s="20">
+        <v>3</v>
+      </c>
+      <c r="N374" s="20">
+        <v>100</v>
+      </c>
+      <c r="P374" s="20" t="s">
+        <v>2020</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="B4:P373">
+  <conditionalFormatting sqref="B4:P374">
     <cfRule type="containsBlanks" dxfId="11" priority="1">
       <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>

</xml_diff>

<commit_message>
add the item rare dada
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/HItem.xlsx
+++ b/ConfigData/Xlsx/HItem.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="材料" sheetId="1" r:id="rId1"/>
@@ -217,7 +217,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3533" uniqueCount="1996">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3533" uniqueCount="1997">
   <si>
     <t>血蓟</t>
   </si>
@@ -6872,6 +6872,10 @@
   </si>
   <si>
     <t>zygu3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>一种生活在湖中的鱼类</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -7751,7 +7755,275 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="66">
+  <dxfs count="84">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -7872,33 +8144,6 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -8407,33 +8652,6 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -9083,33 +9301,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <border outline="0">
         <left style="thin">
           <color theme="4"/>
@@ -9165,13 +9356,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -9186,87 +9370,87 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:Q374" totalsRowShown="0" headerRowDxfId="64" dataDxfId="63" tableBorderDxfId="62">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:Q374" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82" tableBorderDxfId="81">
   <autoFilter ref="A3:Q374"/>
   <sortState ref="A4:Q347">
     <sortCondition ref="A3:A347"/>
   </sortState>
   <tableColumns count="17">
-    <tableColumn id="1" name="Id" dataDxfId="61"/>
-    <tableColumn id="2" name="Name" dataDxfId="60"/>
+    <tableColumn id="1" name="Id" dataDxfId="80"/>
+    <tableColumn id="2" name="Name" dataDxfId="79"/>
     <tableColumn id="10" name="Ename"/>
-    <tableColumn id="3" name="Type" dataDxfId="59"/>
+    <tableColumn id="3" name="Type" dataDxfId="78"/>
     <tableColumn id="13" name="SubType"/>
-    <tableColumn id="4" name="Descript" dataDxfId="58"/>
-    <tableColumn id="5" name="Level" dataDxfId="57"/>
-    <tableColumn id="6" name="Rare" dataDxfId="56"/>
-    <tableColumn id="7" name="MaxPile" dataDxfId="55"/>
-    <tableColumn id="8" name="ValueFactor" dataDxfId="54"/>
-    <tableColumn id="11" name="IsUsable" dataDxfId="53"/>
-    <tableColumn id="12" name="IsThrowable" dataDxfId="52"/>
-    <tableColumn id="17" name="ShowCollectTip" dataDxfId="51"/>
+    <tableColumn id="4" name="Descript" dataDxfId="77"/>
+    <tableColumn id="5" name="Level" dataDxfId="76"/>
+    <tableColumn id="6" name="Rare" dataDxfId="14"/>
+    <tableColumn id="7" name="MaxPile" dataDxfId="75"/>
+    <tableColumn id="8" name="ValueFactor" dataDxfId="74"/>
+    <tableColumn id="11" name="IsUsable" dataDxfId="73"/>
+    <tableColumn id="12" name="IsThrowable" dataDxfId="72"/>
+    <tableColumn id="17" name="ShowCollectTip" dataDxfId="71"/>
     <tableColumn id="16" name="RandomGroup"/>
-    <tableColumn id="15" name="Frequency" dataDxfId="50"/>
+    <tableColumn id="15" name="Frequency" dataDxfId="70"/>
     <tableColumn id="9" name="Attributes"/>
-    <tableColumn id="14" name="Url" dataDxfId="49"/>
+    <tableColumn id="14" name="Url" dataDxfId="69"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A3:Q20" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42" tableBorderDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A3:Q20" totalsRowShown="0" headerRowDxfId="63" dataDxfId="62" tableBorderDxfId="61">
   <autoFilter ref="A3:Q20"/>
   <sortState ref="A4:R435">
     <sortCondition ref="A3:A435"/>
   </sortState>
   <tableColumns count="17">
-    <tableColumn id="1" name="Id" dataDxfId="40"/>
-    <tableColumn id="2" name="Name" dataDxfId="39"/>
-    <tableColumn id="10" name="Ename" dataDxfId="38"/>
-    <tableColumn id="3" name="Type" dataDxfId="37"/>
-    <tableColumn id="13" name="SubType" dataDxfId="36"/>
-    <tableColumn id="4" name="Descript" dataDxfId="35"/>
-    <tableColumn id="5" name="Level" dataDxfId="34"/>
-    <tableColumn id="6" name="Rare" dataDxfId="33"/>
-    <tableColumn id="7" name="MaxPile" dataDxfId="32"/>
-    <tableColumn id="8" name="ValueFactor" dataDxfId="31"/>
-    <tableColumn id="11" name="IsUsable" dataDxfId="30"/>
-    <tableColumn id="12" name="IsThrowable" dataDxfId="29"/>
-    <tableColumn id="17" name="ShowCollectTip" dataDxfId="28"/>
-    <tableColumn id="16" name="RandomGroup" dataDxfId="27"/>
-    <tableColumn id="15" name="Frequency" dataDxfId="26"/>
-    <tableColumn id="9" name="Attributes" dataDxfId="25"/>
-    <tableColumn id="14" name="Url" dataDxfId="24"/>
+    <tableColumn id="1" name="Id" dataDxfId="60"/>
+    <tableColumn id="2" name="Name" dataDxfId="59"/>
+    <tableColumn id="10" name="Ename" dataDxfId="58"/>
+    <tableColumn id="3" name="Type" dataDxfId="57"/>
+    <tableColumn id="13" name="SubType" dataDxfId="56"/>
+    <tableColumn id="4" name="Descript" dataDxfId="55"/>
+    <tableColumn id="5" name="Level" dataDxfId="54"/>
+    <tableColumn id="6" name="Rare" dataDxfId="7"/>
+    <tableColumn id="7" name="MaxPile" dataDxfId="53"/>
+    <tableColumn id="8" name="ValueFactor" dataDxfId="52"/>
+    <tableColumn id="11" name="IsUsable" dataDxfId="51"/>
+    <tableColumn id="12" name="IsThrowable" dataDxfId="50"/>
+    <tableColumn id="17" name="ShowCollectTip" dataDxfId="49"/>
+    <tableColumn id="16" name="RandomGroup" dataDxfId="48"/>
+    <tableColumn id="15" name="Frequency" dataDxfId="47"/>
+    <tableColumn id="9" name="Attributes" dataDxfId="46"/>
+    <tableColumn id="14" name="Url" dataDxfId="45"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表1_34" displayName="表1_34" ref="A3:Q121" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16" tableBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表1_34" displayName="表1_34" ref="A3:Q121" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37" tableBorderDxfId="36">
   <autoFilter ref="A3:Q121"/>
   <sortState ref="A4:Q121">
     <sortCondition ref="A3:A121"/>
   </sortState>
   <tableColumns count="17">
-    <tableColumn id="1" name="Id" dataDxfId="14"/>
-    <tableColumn id="2" name="Name" dataDxfId="13"/>
-    <tableColumn id="10" name="Ename" dataDxfId="12"/>
-    <tableColumn id="3" name="Type" dataDxfId="11"/>
-    <tableColumn id="13" name="SubType" dataDxfId="10"/>
-    <tableColumn id="4" name="Descript" dataDxfId="9"/>
-    <tableColumn id="5" name="Level" dataDxfId="8"/>
-    <tableColumn id="6" name="Rare" dataDxfId="7"/>
-    <tableColumn id="7" name="MaxPile" dataDxfId="6"/>
-    <tableColumn id="8" name="ValueFactor" dataDxfId="5"/>
-    <tableColumn id="11" name="IsUsable" dataDxfId="4"/>
-    <tableColumn id="12" name="IsThrowable" dataDxfId="3"/>
+    <tableColumn id="1" name="Id" dataDxfId="35"/>
+    <tableColumn id="2" name="Name" dataDxfId="34"/>
+    <tableColumn id="10" name="Ename" dataDxfId="33"/>
+    <tableColumn id="3" name="Type" dataDxfId="32"/>
+    <tableColumn id="13" name="SubType" dataDxfId="31"/>
+    <tableColumn id="4" name="Descript" dataDxfId="30"/>
+    <tableColumn id="5" name="Level" dataDxfId="29"/>
+    <tableColumn id="6" name="Rare" dataDxfId="0"/>
+    <tableColumn id="7" name="MaxPile" dataDxfId="28"/>
+    <tableColumn id="8" name="ValueFactor" dataDxfId="27"/>
+    <tableColumn id="11" name="IsUsable" dataDxfId="26"/>
+    <tableColumn id="12" name="IsThrowable" dataDxfId="25"/>
     <tableColumn id="17" name="ShowCollectTip"/>
     <tableColumn id="16" name="RandomGroup"/>
-    <tableColumn id="15" name="Frequency" dataDxfId="2"/>
-    <tableColumn id="9" name="Attributes" dataDxfId="1"/>
-    <tableColumn id="14" name="Url" dataDxfId="0"/>
+    <tableColumn id="15" name="Frequency" dataDxfId="24"/>
+    <tableColumn id="9" name="Attributes" dataDxfId="23"/>
+    <tableColumn id="14" name="Url" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9595,11 +9779,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q374"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="Q4" sqref="Q4:Q34"/>
+      <selection pane="bottomRight" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -10470,8 +10654,8 @@
       <c r="E17" s="20">
         <v>10</v>
       </c>
-      <c r="F17" s="20" t="s">
-        <v>19</v>
+      <c r="F17" s="31" t="s">
+        <v>1996</v>
       </c>
       <c r="G17" s="20">
         <v>1</v>
@@ -27318,7 +27502,7 @@
       <c r="G356" s="30">
         <v>1</v>
       </c>
-      <c r="H356" s="30">
+      <c r="H356" s="20">
         <v>1</v>
       </c>
       <c r="I356" s="30">
@@ -27365,7 +27549,7 @@
       <c r="G357" s="30">
         <v>1</v>
       </c>
-      <c r="H357" s="30">
+      <c r="H357" s="20">
         <v>1</v>
       </c>
       <c r="I357" s="30">
@@ -27412,7 +27596,7 @@
       <c r="G358" s="30">
         <v>1</v>
       </c>
-      <c r="H358" s="30">
+      <c r="H358" s="20">
         <v>1</v>
       </c>
       <c r="I358" s="30">
@@ -27459,7 +27643,7 @@
       <c r="G359" s="30">
         <v>1</v>
       </c>
-      <c r="H359" s="30">
+      <c r="H359" s="20">
         <v>1</v>
       </c>
       <c r="I359" s="30">
@@ -27506,7 +27690,7 @@
       <c r="G360" s="30">
         <v>1</v>
       </c>
-      <c r="H360" s="30">
+      <c r="H360" s="20">
         <v>4</v>
       </c>
       <c r="I360" s="30">
@@ -27553,7 +27737,7 @@
       <c r="G361" s="30">
         <v>1</v>
       </c>
-      <c r="H361" s="30">
+      <c r="H361" s="20">
         <v>4</v>
       </c>
       <c r="I361" s="30">
@@ -27600,7 +27784,7 @@
       <c r="G362" s="30">
         <v>1</v>
       </c>
-      <c r="H362" s="30">
+      <c r="H362" s="20">
         <v>4</v>
       </c>
       <c r="I362" s="30">
@@ -27647,7 +27831,7 @@
       <c r="G363" s="30">
         <v>1</v>
       </c>
-      <c r="H363" s="30">
+      <c r="H363" s="20">
         <v>3</v>
       </c>
       <c r="I363" s="30">
@@ -27694,7 +27878,7 @@
       <c r="G364" s="30">
         <v>1</v>
       </c>
-      <c r="H364" s="30">
+      <c r="H364" s="20">
         <v>3</v>
       </c>
       <c r="I364" s="30">
@@ -27741,7 +27925,7 @@
       <c r="G365" s="30">
         <v>1</v>
       </c>
-      <c r="H365" s="30">
+      <c r="H365" s="20">
         <v>3</v>
       </c>
       <c r="I365" s="30">
@@ -27788,7 +27972,7 @@
       <c r="G366" s="30">
         <v>1</v>
       </c>
-      <c r="H366" s="30">
+      <c r="H366" s="20">
         <v>5</v>
       </c>
       <c r="I366" s="30">
@@ -27835,7 +28019,7 @@
       <c r="G367" s="30">
         <v>1</v>
       </c>
-      <c r="H367" s="30">
+      <c r="H367" s="20">
         <v>2</v>
       </c>
       <c r="I367" s="30">
@@ -27882,7 +28066,7 @@
       <c r="G368" s="30">
         <v>1</v>
       </c>
-      <c r="H368" s="30">
+      <c r="H368" s="20">
         <v>2</v>
       </c>
       <c r="I368" s="30">
@@ -27929,7 +28113,7 @@
       <c r="G369" s="30">
         <v>1</v>
       </c>
-      <c r="H369" s="30">
+      <c r="H369" s="20">
         <v>2</v>
       </c>
       <c r="I369" s="30">
@@ -27976,7 +28160,7 @@
       <c r="G370" s="30">
         <v>1</v>
       </c>
-      <c r="H370" s="30">
+      <c r="H370" s="20">
         <v>5</v>
       </c>
       <c r="I370" s="30">
@@ -28023,7 +28207,7 @@
       <c r="G371" s="30">
         <v>1</v>
       </c>
-      <c r="H371" s="30">
+      <c r="H371" s="20">
         <v>5</v>
       </c>
       <c r="I371" s="30">
@@ -28070,7 +28254,7 @@
       <c r="G372" s="30">
         <v>1</v>
       </c>
-      <c r="H372" s="30">
+      <c r="H372" s="20">
         <v>6</v>
       </c>
       <c r="I372" s="30">
@@ -28117,7 +28301,7 @@
       <c r="G373" s="30">
         <v>1</v>
       </c>
-      <c r="H373" s="30">
+      <c r="H373" s="20">
         <v>6</v>
       </c>
       <c r="I373" s="30">
@@ -28164,7 +28348,7 @@
       <c r="G374" s="30">
         <v>1</v>
       </c>
-      <c r="H374" s="30">
+      <c r="H374" s="20">
         <v>4</v>
       </c>
       <c r="I374" s="30">
@@ -28192,8 +28376,27 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="B4:Q374">
-    <cfRule type="containsBlanks" dxfId="65" priority="1">
+    <cfRule type="containsBlanks" dxfId="21" priority="6">
       <formula>LEN(TRIM(B4))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H4:H374">
+    <cfRule type="cellIs" dxfId="17" priority="5" operator="between">
+      <formula>1</formula>
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="4" operator="between">
+      <formula>3</formula>
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="3" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="2" operator="equal">
+      <formula>6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="1" operator="equal">
+      <formula>7</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -28209,18 +28412,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="M1" sqref="M1:M3"/>
+      <selection pane="bottomRight" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
     <col min="4" max="5" width="3.25" customWidth="1"/>
-    <col min="6" max="6" width="34" customWidth="1"/>
+    <col min="6" max="6" width="29.875" customWidth="1"/>
     <col min="7" max="9" width="5.75" customWidth="1"/>
     <col min="10" max="13" width="6.5" customWidth="1"/>
     <col min="14" max="14" width="4.375" customWidth="1"/>
@@ -28409,6 +28612,7 @@
       <c r="G4">
         <v>1</v>
       </c>
+      <c r="H4" s="20"/>
       <c r="I4">
         <v>1</v>
       </c>
@@ -28444,6 +28648,7 @@
       <c r="G5">
         <v>1</v>
       </c>
+      <c r="H5" s="20"/>
       <c r="I5">
         <v>1</v>
       </c>
@@ -28479,6 +28684,7 @@
       <c r="G6">
         <v>1</v>
       </c>
+      <c r="H6" s="20"/>
       <c r="I6">
         <v>1</v>
       </c>
@@ -28514,6 +28720,7 @@
       <c r="G7">
         <v>1</v>
       </c>
+      <c r="H7" s="20"/>
       <c r="I7">
         <v>1</v>
       </c>
@@ -28549,6 +28756,7 @@
       <c r="G8">
         <v>1</v>
       </c>
+      <c r="H8" s="20"/>
       <c r="I8">
         <v>1</v>
       </c>
@@ -28584,6 +28792,7 @@
       <c r="G9">
         <v>1</v>
       </c>
+      <c r="H9" s="20"/>
       <c r="I9">
         <v>1</v>
       </c>
@@ -28619,6 +28828,7 @@
       <c r="G10">
         <v>1</v>
       </c>
+      <c r="H10" s="20"/>
       <c r="I10">
         <v>1</v>
       </c>
@@ -28654,6 +28864,7 @@
       <c r="G11">
         <v>1</v>
       </c>
+      <c r="H11" s="20"/>
       <c r="I11">
         <v>1</v>
       </c>
@@ -28689,6 +28900,7 @@
       <c r="G12">
         <v>1</v>
       </c>
+      <c r="H12" s="20"/>
       <c r="I12">
         <v>1</v>
       </c>
@@ -28724,6 +28936,7 @@
       <c r="G13">
         <v>1</v>
       </c>
+      <c r="H13" s="20"/>
       <c r="I13">
         <v>1</v>
       </c>
@@ -28759,6 +28972,7 @@
       <c r="G14">
         <v>1</v>
       </c>
+      <c r="H14" s="20"/>
       <c r="I14">
         <v>1</v>
       </c>
@@ -28794,7 +29008,7 @@
       <c r="G15" s="7">
         <v>1</v>
       </c>
-      <c r="H15" s="7"/>
+      <c r="H15" s="20"/>
       <c r="I15" s="7">
         <v>99</v>
       </c>
@@ -28834,7 +29048,7 @@
       <c r="G16" s="8">
         <v>1</v>
       </c>
-      <c r="H16" s="8"/>
+      <c r="H16" s="20"/>
       <c r="I16" s="8">
         <v>99</v>
       </c>
@@ -28874,7 +29088,7 @@
       <c r="G17" s="8">
         <v>1</v>
       </c>
-      <c r="H17" s="8"/>
+      <c r="H17" s="20"/>
       <c r="I17" s="8">
         <v>99</v>
       </c>
@@ -28914,7 +29128,7 @@
       <c r="G18" s="8">
         <v>1</v>
       </c>
-      <c r="H18" s="8"/>
+      <c r="H18" s="20"/>
       <c r="I18" s="8">
         <v>99</v>
       </c>
@@ -28954,7 +29168,7 @@
       <c r="G19" s="8">
         <v>1</v>
       </c>
-      <c r="H19" s="8"/>
+      <c r="H19" s="20"/>
       <c r="I19" s="8">
         <v>99</v>
       </c>
@@ -28994,7 +29208,7 @@
       <c r="G20" s="8">
         <v>1</v>
       </c>
-      <c r="H20" s="8"/>
+      <c r="H20" s="20"/>
       <c r="I20" s="8">
         <v>99</v>
       </c>
@@ -29015,28 +29229,52 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="B6:Q20 B5:D5 L5:P5 F5:J5">
-    <cfRule type="containsBlanks" dxfId="48" priority="6">
+    <cfRule type="containsBlanks" dxfId="68" priority="12">
       <formula>LEN(TRIM(B5))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B4:Q4">
-    <cfRule type="containsBlanks" dxfId="47" priority="4">
+  <conditionalFormatting sqref="B4:G4 I4:Q4">
+    <cfRule type="containsBlanks" dxfId="67" priority="10">
       <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q5">
-    <cfRule type="containsBlanks" dxfId="46" priority="3">
+    <cfRule type="containsBlanks" dxfId="66" priority="9">
       <formula>LEN(TRIM(Q5))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="containsBlanks" dxfId="45" priority="2">
+    <cfRule type="containsBlanks" dxfId="65" priority="8">
       <formula>LEN(TRIM(K5))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="containsBlanks" dxfId="44" priority="1">
+    <cfRule type="containsBlanks" dxfId="64" priority="7">
       <formula>LEN(TRIM(E5))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H4:H20">
+    <cfRule type="containsBlanks" dxfId="13" priority="6">
+      <formula>LEN(TRIM(H4))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H4:H20">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+      <formula>7</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
+      <formula>6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="4" operator="between">
+      <formula>3</formula>
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="5" operator="between">
+      <formula>1</formula>
+      <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -29053,19 +29291,19 @@
   <dimension ref="A1:Q121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B100" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="M1" sqref="M1:M3"/>
+      <selection pane="bottomRight" activeCell="G111" sqref="G111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="10.25" customWidth="1"/>
-    <col min="2" max="2" width="14.5" customWidth="1"/>
+    <col min="2" max="2" width="10.625" customWidth="1"/>
     <col min="3" max="3" width="11.125" customWidth="1"/>
     <col min="4" max="5" width="3.75" customWidth="1"/>
-    <col min="6" max="6" width="31" customWidth="1"/>
+    <col min="6" max="6" width="25.875" customWidth="1"/>
     <col min="7" max="9" width="4.875" customWidth="1"/>
     <col min="10" max="13" width="6.5" customWidth="1"/>
     <col min="14" max="16" width="3.75" customWidth="1"/>
@@ -29253,7 +29491,7 @@
       <c r="G4">
         <v>1</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="20">
         <v>3</v>
       </c>
       <c r="I4">
@@ -29291,7 +29529,7 @@
       <c r="G5">
         <v>1</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="20">
         <v>4</v>
       </c>
       <c r="I5">
@@ -29332,7 +29570,7 @@
       <c r="G6">
         <v>1</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="20">
         <v>5</v>
       </c>
       <c r="I6">
@@ -29373,7 +29611,7 @@
       <c r="G7">
         <v>1</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="20">
         <v>6</v>
       </c>
       <c r="I7">
@@ -29414,7 +29652,7 @@
       <c r="G8">
         <v>1</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="20">
         <v>3</v>
       </c>
       <c r="I8">
@@ -29455,7 +29693,7 @@
       <c r="G9">
         <v>1</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="20">
         <v>3</v>
       </c>
       <c r="I9">
@@ -29496,7 +29734,7 @@
       <c r="G10">
         <v>1</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="20">
         <v>3</v>
       </c>
       <c r="I10">
@@ -29537,7 +29775,7 @@
       <c r="G11">
         <v>1</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="20">
         <v>3</v>
       </c>
       <c r="I11">
@@ -29578,7 +29816,7 @@
       <c r="G12">
         <v>1</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="20">
         <v>3</v>
       </c>
       <c r="I12">
@@ -29619,7 +29857,7 @@
       <c r="G13">
         <v>1</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="20">
         <v>3</v>
       </c>
       <c r="I13">
@@ -29660,7 +29898,7 @@
       <c r="G14">
         <v>1</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="20">
         <v>3</v>
       </c>
       <c r="I14">
@@ -29701,7 +29939,7 @@
       <c r="G15">
         <v>1</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="20">
         <v>3</v>
       </c>
       <c r="I15">
@@ -29742,7 +29980,7 @@
       <c r="G16">
         <v>1</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="20">
         <v>3</v>
       </c>
       <c r="I16">
@@ -29783,7 +30021,7 @@
       <c r="G17">
         <v>1</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="20">
         <v>3</v>
       </c>
       <c r="I17">
@@ -29824,7 +30062,7 @@
       <c r="G18">
         <v>1</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="20">
         <v>3</v>
       </c>
       <c r="I18">
@@ -29865,7 +30103,7 @@
       <c r="G19">
         <v>1</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="20">
         <v>3</v>
       </c>
       <c r="I19">
@@ -29906,7 +30144,7 @@
       <c r="G20">
         <v>1</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="20">
         <v>3</v>
       </c>
       <c r="I20">
@@ -29947,7 +30185,7 @@
       <c r="G21">
         <v>1</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="20">
         <v>3</v>
       </c>
       <c r="I21">
@@ -29988,7 +30226,7 @@
       <c r="G22">
         <v>1</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="20">
         <v>3</v>
       </c>
       <c r="I22">
@@ -30029,7 +30267,7 @@
       <c r="G23">
         <v>1</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="20">
         <v>3</v>
       </c>
       <c r="I23">
@@ -30070,7 +30308,7 @@
       <c r="G24">
         <v>1</v>
       </c>
-      <c r="H24">
+      <c r="H24" s="20">
         <v>3</v>
       </c>
       <c r="I24">
@@ -30111,7 +30349,7 @@
       <c r="G25">
         <v>1</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="20">
         <v>3</v>
       </c>
       <c r="I25">
@@ -30152,7 +30390,7 @@
       <c r="G26">
         <v>1</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="20">
         <v>3</v>
       </c>
       <c r="I26">
@@ -30193,7 +30431,7 @@
       <c r="G27">
         <v>1</v>
       </c>
-      <c r="H27">
+      <c r="H27" s="20">
         <v>3</v>
       </c>
       <c r="I27">
@@ -30234,7 +30472,7 @@
       <c r="G28">
         <v>1</v>
       </c>
-      <c r="H28">
+      <c r="H28" s="20">
         <v>3</v>
       </c>
       <c r="I28">
@@ -30275,7 +30513,7 @@
       <c r="G29">
         <v>1</v>
       </c>
-      <c r="H29">
+      <c r="H29" s="20">
         <v>3</v>
       </c>
       <c r="I29">
@@ -30316,7 +30554,7 @@
       <c r="G30">
         <v>1</v>
       </c>
-      <c r="H30">
+      <c r="H30" s="20">
         <v>3</v>
       </c>
       <c r="I30">
@@ -30357,7 +30595,7 @@
       <c r="G31">
         <v>1</v>
       </c>
-      <c r="H31">
+      <c r="H31" s="20">
         <v>3</v>
       </c>
       <c r="I31">
@@ -30398,7 +30636,7 @@
       <c r="G32">
         <v>1</v>
       </c>
-      <c r="H32">
+      <c r="H32" s="20">
         <v>3</v>
       </c>
       <c r="I32">
@@ -30439,7 +30677,7 @@
       <c r="G33">
         <v>1</v>
       </c>
-      <c r="H33">
+      <c r="H33" s="20">
         <v>3</v>
       </c>
       <c r="I33">
@@ -30480,7 +30718,7 @@
       <c r="G34">
         <v>1</v>
       </c>
-      <c r="H34" s="15">
+      <c r="H34" s="20">
         <v>3</v>
       </c>
       <c r="I34">
@@ -30521,7 +30759,7 @@
       <c r="G35">
         <v>1</v>
       </c>
-      <c r="H35" s="15">
+      <c r="H35" s="20">
         <v>3</v>
       </c>
       <c r="I35">
@@ -30562,7 +30800,7 @@
       <c r="G36">
         <v>1</v>
       </c>
-      <c r="H36" s="15">
+      <c r="H36" s="20">
         <v>3</v>
       </c>
       <c r="I36">
@@ -30603,7 +30841,7 @@
       <c r="G37">
         <v>1</v>
       </c>
-      <c r="H37" s="15">
+      <c r="H37" s="20">
         <v>3</v>
       </c>
       <c r="I37">
@@ -30644,7 +30882,7 @@
       <c r="G38">
         <v>1</v>
       </c>
-      <c r="H38" s="6">
+      <c r="H38" s="20">
         <v>3</v>
       </c>
       <c r="I38">
@@ -30685,7 +30923,7 @@
       <c r="G39">
         <v>1</v>
       </c>
-      <c r="H39" s="14">
+      <c r="H39" s="20">
         <v>1</v>
       </c>
       <c r="I39">
@@ -30726,7 +30964,7 @@
       <c r="G40">
         <v>1</v>
       </c>
-      <c r="H40" s="14">
+      <c r="H40" s="20">
         <v>2</v>
       </c>
       <c r="I40">
@@ -30767,7 +31005,7 @@
       <c r="G41">
         <v>1</v>
       </c>
-      <c r="H41" s="14">
+      <c r="H41" s="20">
         <v>4</v>
       </c>
       <c r="I41">
@@ -30808,7 +31046,7 @@
       <c r="G42">
         <v>1</v>
       </c>
-      <c r="H42" s="14">
+      <c r="H42" s="20">
         <v>6</v>
       </c>
       <c r="I42">
@@ -30849,7 +31087,7 @@
       <c r="G43">
         <v>1</v>
       </c>
-      <c r="H43" s="6">
+      <c r="H43" s="20">
         <v>3</v>
       </c>
       <c r="I43">
@@ -30890,7 +31128,7 @@
       <c r="G44">
         <v>1</v>
       </c>
-      <c r="H44" s="6">
+      <c r="H44" s="20">
         <v>3</v>
       </c>
       <c r="I44">
@@ -30931,7 +31169,7 @@
       <c r="G45">
         <v>1</v>
       </c>
-      <c r="H45" s="6">
+      <c r="H45" s="20">
         <v>3</v>
       </c>
       <c r="I45">
@@ -30972,7 +31210,7 @@
       <c r="G46">
         <v>1</v>
       </c>
-      <c r="H46" s="6">
+      <c r="H46" s="20">
         <v>3</v>
       </c>
       <c r="I46">
@@ -31013,7 +31251,7 @@
       <c r="G47">
         <v>1</v>
       </c>
-      <c r="H47" s="6">
+      <c r="H47" s="20">
         <v>3</v>
       </c>
       <c r="I47">
@@ -31054,7 +31292,7 @@
       <c r="G48">
         <v>1</v>
       </c>
-      <c r="H48" s="6">
+      <c r="H48" s="20">
         <v>3</v>
       </c>
       <c r="I48">
@@ -31095,7 +31333,7 @@
       <c r="G49">
         <v>1</v>
       </c>
-      <c r="H49" s="6">
+      <c r="H49" s="20">
         <v>3</v>
       </c>
       <c r="I49">
@@ -31136,7 +31374,7 @@
       <c r="G50">
         <v>1</v>
       </c>
-      <c r="H50" s="6">
+      <c r="H50" s="20">
         <v>3</v>
       </c>
       <c r="I50">
@@ -31177,7 +31415,7 @@
       <c r="G51">
         <v>1</v>
       </c>
-      <c r="H51" s="6">
+      <c r="H51" s="20">
         <v>3</v>
       </c>
       <c r="I51">
@@ -31218,7 +31456,7 @@
       <c r="G52">
         <v>1</v>
       </c>
-      <c r="H52" s="6">
+      <c r="H52" s="20">
         <v>3</v>
       </c>
       <c r="I52">
@@ -31259,7 +31497,7 @@
       <c r="G53">
         <v>1</v>
       </c>
-      <c r="H53" s="6">
+      <c r="H53" s="20">
         <v>3</v>
       </c>
       <c r="I53">
@@ -31300,7 +31538,7 @@
       <c r="G54">
         <v>1</v>
       </c>
-      <c r="H54" s="6">
+      <c r="H54" s="20">
         <v>3</v>
       </c>
       <c r="I54">
@@ -31341,7 +31579,7 @@
       <c r="G55">
         <v>1</v>
       </c>
-      <c r="H55" s="6">
+      <c r="H55" s="20">
         <v>3</v>
       </c>
       <c r="I55">
@@ -31382,7 +31620,7 @@
       <c r="G56">
         <v>1</v>
       </c>
-      <c r="H56" s="6">
+      <c r="H56" s="20">
         <v>3</v>
       </c>
       <c r="I56">
@@ -31423,7 +31661,7 @@
       <c r="G57">
         <v>1</v>
       </c>
-      <c r="H57" s="6">
+      <c r="H57" s="20">
         <v>3</v>
       </c>
       <c r="I57">
@@ -31464,7 +31702,7 @@
       <c r="G58">
         <v>1</v>
       </c>
-      <c r="H58" s="6">
+      <c r="H58" s="20">
         <v>3</v>
       </c>
       <c r="I58">
@@ -31505,7 +31743,7 @@
       <c r="G59">
         <v>1</v>
       </c>
-      <c r="H59" s="6">
+      <c r="H59" s="20">
         <v>3</v>
       </c>
       <c r="I59">
@@ -31546,7 +31784,7 @@
       <c r="G60">
         <v>1</v>
       </c>
-      <c r="H60" s="6">
+      <c r="H60" s="20">
         <v>3</v>
       </c>
       <c r="I60">
@@ -31587,7 +31825,7 @@
       <c r="G61">
         <v>1</v>
       </c>
-      <c r="H61" s="6">
+      <c r="H61" s="20">
         <v>3</v>
       </c>
       <c r="I61">
@@ -31628,7 +31866,7 @@
       <c r="G62">
         <v>1</v>
       </c>
-      <c r="H62" s="6">
+      <c r="H62" s="20">
         <v>3</v>
       </c>
       <c r="I62">
@@ -31669,7 +31907,7 @@
       <c r="G63">
         <v>1</v>
       </c>
-      <c r="H63" s="6">
+      <c r="H63" s="20">
         <v>3</v>
       </c>
       <c r="I63">
@@ -31710,7 +31948,7 @@
       <c r="G64">
         <v>1</v>
       </c>
-      <c r="H64" s="6">
+      <c r="H64" s="20">
         <v>3</v>
       </c>
       <c r="I64">
@@ -31751,7 +31989,7 @@
       <c r="G65">
         <v>1</v>
       </c>
-      <c r="H65" s="6">
+      <c r="H65" s="20">
         <v>3</v>
       </c>
       <c r="I65">
@@ -31792,7 +32030,7 @@
       <c r="G66">
         <v>1</v>
       </c>
-      <c r="H66">
+      <c r="H66" s="20">
         <v>4</v>
       </c>
       <c r="I66">
@@ -31830,7 +32068,7 @@
       <c r="G67">
         <v>1</v>
       </c>
-      <c r="H67">
+      <c r="H67" s="20">
         <v>4</v>
       </c>
       <c r="I67">
@@ -31868,7 +32106,7 @@
       <c r="G68">
         <v>1</v>
       </c>
-      <c r="H68">
+      <c r="H68" s="20">
         <v>4</v>
       </c>
       <c r="I68">
@@ -31906,7 +32144,7 @@
       <c r="G69">
         <v>1</v>
       </c>
-      <c r="H69">
+      <c r="H69" s="20">
         <v>4</v>
       </c>
       <c r="I69">
@@ -31944,7 +32182,7 @@
       <c r="G70">
         <v>1</v>
       </c>
-      <c r="H70">
+      <c r="H70" s="20">
         <v>4</v>
       </c>
       <c r="I70">
@@ -31982,7 +32220,7 @@
       <c r="G71">
         <v>1</v>
       </c>
-      <c r="H71">
+      <c r="H71" s="20">
         <v>4</v>
       </c>
       <c r="I71">
@@ -32020,7 +32258,7 @@
       <c r="G72">
         <v>1</v>
       </c>
-      <c r="H72">
+      <c r="H72" s="20">
         <v>4</v>
       </c>
       <c r="I72">
@@ -32058,7 +32296,7 @@
       <c r="G73">
         <v>1</v>
       </c>
-      <c r="H73">
+      <c r="H73" s="20">
         <v>4</v>
       </c>
       <c r="I73">
@@ -32096,7 +32334,7 @@
       <c r="G74">
         <v>1</v>
       </c>
-      <c r="H74">
+      <c r="H74" s="20">
         <v>2</v>
       </c>
       <c r="I74">
@@ -32134,7 +32372,7 @@
       <c r="G75">
         <v>1</v>
       </c>
-      <c r="H75">
+      <c r="H75" s="20">
         <v>2</v>
       </c>
       <c r="I75">
@@ -32172,7 +32410,7 @@
       <c r="G76">
         <v>1</v>
       </c>
-      <c r="H76">
+      <c r="H76" s="20">
         <v>2</v>
       </c>
       <c r="I76">
@@ -32210,7 +32448,7 @@
       <c r="G77">
         <v>1</v>
       </c>
-      <c r="H77">
+      <c r="H77" s="20">
         <v>2</v>
       </c>
       <c r="I77">
@@ -32248,7 +32486,7 @@
       <c r="G78">
         <v>1</v>
       </c>
-      <c r="H78">
+      <c r="H78" s="20">
         <v>2</v>
       </c>
       <c r="I78">
@@ -32286,7 +32524,7 @@
       <c r="G79">
         <v>1</v>
       </c>
-      <c r="H79">
+      <c r="H79" s="20">
         <v>2</v>
       </c>
       <c r="I79">
@@ -32324,6 +32562,7 @@
       <c r="G80">
         <v>1</v>
       </c>
+      <c r="H80" s="20"/>
       <c r="I80">
         <v>99</v>
       </c>
@@ -32362,6 +32601,7 @@
       <c r="G81">
         <v>1</v>
       </c>
+      <c r="H81" s="20"/>
       <c r="I81">
         <v>99</v>
       </c>
@@ -32400,6 +32640,7 @@
       <c r="G82">
         <v>1</v>
       </c>
+      <c r="H82" s="20"/>
       <c r="I82">
         <v>99</v>
       </c>
@@ -32438,6 +32679,7 @@
       <c r="G83">
         <v>1</v>
       </c>
+      <c r="H83" s="20"/>
       <c r="I83">
         <v>99</v>
       </c>
@@ -32476,6 +32718,7 @@
       <c r="G84">
         <v>1</v>
       </c>
+      <c r="H84" s="20"/>
       <c r="I84">
         <v>99</v>
       </c>
@@ -32514,6 +32757,7 @@
       <c r="G85">
         <v>1</v>
       </c>
+      <c r="H85" s="20"/>
       <c r="I85">
         <v>99</v>
       </c>
@@ -32552,6 +32796,7 @@
       <c r="G86">
         <v>1</v>
       </c>
+      <c r="H86" s="20"/>
       <c r="I86">
         <v>99</v>
       </c>
@@ -32590,6 +32835,7 @@
       <c r="G87">
         <v>1</v>
       </c>
+      <c r="H87" s="20"/>
       <c r="I87">
         <v>99</v>
       </c>
@@ -32628,7 +32874,7 @@
       <c r="G88">
         <v>1</v>
       </c>
-      <c r="H88">
+      <c r="H88" s="20">
         <v>2</v>
       </c>
       <c r="I88">
@@ -32669,7 +32915,7 @@
       <c r="G89">
         <v>1</v>
       </c>
-      <c r="H89">
+      <c r="H89" s="20">
         <v>3</v>
       </c>
       <c r="I89">
@@ -32710,7 +32956,7 @@
       <c r="G90">
         <v>1</v>
       </c>
-      <c r="H90">
+      <c r="H90" s="20">
         <v>4</v>
       </c>
       <c r="I90">
@@ -32751,7 +32997,7 @@
       <c r="G91">
         <v>1</v>
       </c>
-      <c r="H91">
+      <c r="H91" s="20">
         <v>2</v>
       </c>
       <c r="I91">
@@ -32792,7 +33038,7 @@
       <c r="G92">
         <v>1</v>
       </c>
-      <c r="H92">
+      <c r="H92" s="20">
         <v>3</v>
       </c>
       <c r="I92">
@@ -32833,7 +33079,7 @@
       <c r="G93">
         <v>1</v>
       </c>
-      <c r="H93">
+      <c r="H93" s="20">
         <v>4</v>
       </c>
       <c r="I93">
@@ -32874,7 +33120,7 @@
       <c r="G94">
         <v>1</v>
       </c>
-      <c r="H94">
+      <c r="H94" s="20">
         <v>2</v>
       </c>
       <c r="I94">
@@ -32915,7 +33161,7 @@
       <c r="G95">
         <v>1</v>
       </c>
-      <c r="H95">
+      <c r="H95" s="20">
         <v>3</v>
       </c>
       <c r="I95">
@@ -32956,7 +33202,7 @@
       <c r="G96">
         <v>1</v>
       </c>
-      <c r="H96">
+      <c r="H96" s="20">
         <v>4</v>
       </c>
       <c r="I96">
@@ -32997,7 +33243,7 @@
       <c r="G97">
         <v>1</v>
       </c>
-      <c r="H97">
+      <c r="H97" s="20">
         <v>3</v>
       </c>
       <c r="I97">
@@ -33038,7 +33284,7 @@
       <c r="G98">
         <v>1</v>
       </c>
-      <c r="H98">
+      <c r="H98" s="20">
         <v>3</v>
       </c>
       <c r="I98">
@@ -33079,7 +33325,7 @@
       <c r="G99">
         <v>1</v>
       </c>
-      <c r="H99">
+      <c r="H99" s="20">
         <v>3</v>
       </c>
       <c r="I99">
@@ -33120,7 +33366,7 @@
       <c r="G100">
         <v>1</v>
       </c>
-      <c r="H100">
+      <c r="H100" s="20">
         <v>7</v>
       </c>
       <c r="I100">
@@ -33161,7 +33407,7 @@
       <c r="G101">
         <v>1</v>
       </c>
-      <c r="H101">
+      <c r="H101" s="20">
         <v>4</v>
       </c>
       <c r="I101">
@@ -33202,7 +33448,7 @@
       <c r="G102">
         <v>1</v>
       </c>
-      <c r="H102">
+      <c r="H102" s="20">
         <v>5</v>
       </c>
       <c r="I102">
@@ -33243,7 +33489,7 @@
       <c r="G103">
         <v>1</v>
       </c>
-      <c r="H103">
+      <c r="H103" s="20">
         <v>3</v>
       </c>
       <c r="I103">
@@ -33284,7 +33530,7 @@
       <c r="G104">
         <v>1</v>
       </c>
-      <c r="H104">
+      <c r="H104" s="20">
         <v>4</v>
       </c>
       <c r="I104">
@@ -33325,7 +33571,7 @@
       <c r="G105">
         <v>1</v>
       </c>
-      <c r="H105">
+      <c r="H105" s="20">
         <v>5</v>
       </c>
       <c r="I105">
@@ -33366,7 +33612,7 @@
       <c r="G106">
         <v>1</v>
       </c>
-      <c r="H106">
+      <c r="H106" s="20">
         <v>4</v>
       </c>
       <c r="I106">
@@ -33407,7 +33653,7 @@
       <c r="G107">
         <v>1</v>
       </c>
-      <c r="H107">
+      <c r="H107" s="20">
         <v>6</v>
       </c>
       <c r="I107">
@@ -33448,7 +33694,7 @@
       <c r="G108">
         <v>1</v>
       </c>
-      <c r="H108">
+      <c r="H108" s="20">
         <v>2</v>
       </c>
       <c r="I108">
@@ -33489,7 +33735,7 @@
       <c r="G109">
         <v>1</v>
       </c>
-      <c r="H109">
+      <c r="H109" s="20">
         <v>2</v>
       </c>
       <c r="I109">
@@ -33530,7 +33776,7 @@
       <c r="G110">
         <v>1</v>
       </c>
-      <c r="H110">
+      <c r="H110" s="20">
         <v>2</v>
       </c>
       <c r="I110">
@@ -33571,7 +33817,7 @@
       <c r="G111">
         <v>1</v>
       </c>
-      <c r="H111">
+      <c r="H111" s="20">
         <v>2</v>
       </c>
       <c r="I111">
@@ -33612,7 +33858,7 @@
       <c r="G112" s="14">
         <v>1</v>
       </c>
-      <c r="H112" s="14">
+      <c r="H112" s="20">
         <v>2</v>
       </c>
       <c r="I112">
@@ -33655,7 +33901,7 @@
       <c r="G113" s="14">
         <v>1</v>
       </c>
-      <c r="H113" s="14">
+      <c r="H113" s="20">
         <v>2</v>
       </c>
       <c r="I113">
@@ -33698,7 +33944,7 @@
       <c r="G114" s="14">
         <v>1</v>
       </c>
-      <c r="H114" s="14">
+      <c r="H114" s="20">
         <v>2</v>
       </c>
       <c r="I114">
@@ -33741,7 +33987,7 @@
       <c r="G115">
         <v>1</v>
       </c>
-      <c r="H115">
+      <c r="H115" s="20">
         <v>2</v>
       </c>
       <c r="I115">
@@ -33782,7 +34028,7 @@
       <c r="G116">
         <v>1</v>
       </c>
-      <c r="H116">
+      <c r="H116" s="20">
         <v>2</v>
       </c>
       <c r="I116">
@@ -33823,7 +34069,7 @@
       <c r="G117">
         <v>1</v>
       </c>
-      <c r="H117">
+      <c r="H117" s="20">
         <v>2</v>
       </c>
       <c r="I117">
@@ -33864,7 +34110,7 @@
       <c r="G118">
         <v>1</v>
       </c>
-      <c r="H118">
+      <c r="H118" s="20">
         <v>5</v>
       </c>
       <c r="I118">
@@ -33905,7 +34151,7 @@
       <c r="G119" s="15">
         <v>1</v>
       </c>
-      <c r="H119" s="15">
+      <c r="H119" s="20">
         <v>2</v>
       </c>
       <c r="I119">
@@ -33948,7 +34194,7 @@
       <c r="G120" s="15">
         <v>1</v>
       </c>
-      <c r="H120" s="15">
+      <c r="H120" s="20">
         <v>4</v>
       </c>
       <c r="I120">
@@ -33991,7 +34237,7 @@
       <c r="G121" s="15">
         <v>1</v>
       </c>
-      <c r="H121" s="15">
+      <c r="H121" s="20">
         <v>6</v>
       </c>
       <c r="I121">
@@ -34014,34 +34260,58 @@
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="J97:J113 F109:J114 F9:J11 J5:J21 O8:P21 E5:J8 E115:J121 K5:P7 K8:N37 E4:Q4 E88:J108 K88:Q121 Q5:Q73 K38:P73 E12:J73 E80:Q87">
-    <cfRule type="containsBlanks" dxfId="23" priority="9">
+  <conditionalFormatting sqref="J97:J113 F109:J114 F9:J11 J5:J21 O8:P21 E5:J8 E115:J121 K5:P7 K8:N37 E4:G4 E88:J108 K88:Q121 Q5:Q73 K38:P73 E12:J73 E80:Q87 I4:Q4">
+    <cfRule type="containsBlanks" dxfId="44" priority="15">
       <formula>LEN(TRIM(E4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E109:E111">
-    <cfRule type="containsBlanks" dxfId="22" priority="7">
+    <cfRule type="containsBlanks" dxfId="43" priority="13">
       <formula>LEN(TRIM(E109))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E112:E114">
-    <cfRule type="containsBlanks" dxfId="21" priority="6">
+    <cfRule type="containsBlanks" dxfId="42" priority="12">
       <formula>LEN(TRIM(E112))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9:E11">
-    <cfRule type="containsBlanks" dxfId="20" priority="5">
+    <cfRule type="containsBlanks" dxfId="41" priority="11">
       <formula>LEN(TRIM(E9))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J22:J37 O22:P37">
-    <cfRule type="containsBlanks" dxfId="19" priority="4">
+    <cfRule type="containsBlanks" dxfId="40" priority="10">
       <formula>LEN(TRIM(J22))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E74:Q79">
-    <cfRule type="containsBlanks" dxfId="18" priority="1">
+    <cfRule type="containsBlanks" dxfId="39" priority="7">
       <formula>LEN(TRIM(E74))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H4:H121">
+    <cfRule type="containsBlanks" dxfId="6" priority="6">
+      <formula>LEN(TRIM(H4))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H4:H121">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+      <formula>7</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+      <formula>6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="between">
+      <formula>3</formula>
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="between">
+      <formula>1</formula>
+      <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix the data error
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/HItem.xlsx
+++ b/ConfigData/Xlsx/HItem.xlsx
@@ -7342,442 +7342,6 @@
   <dxfs count="102">
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -8224,6 +7788,110 @@
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="3" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -8708,6 +8376,103 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -9106,6 +8871,241 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -9120,87 +9120,87 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:Q352" totalsRowShown="0" headerRowDxfId="101" dataDxfId="100" tableBorderDxfId="99">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:Q352" totalsRowShown="0" headerRowDxfId="76" dataDxfId="75" tableBorderDxfId="74">
   <autoFilter ref="A3:Q352"/>
   <sortState ref="A4:Q352">
     <sortCondition ref="A3:A352"/>
   </sortState>
   <tableColumns count="17">
-    <tableColumn id="1" name="Id" dataDxfId="98"/>
-    <tableColumn id="2" name="Name" dataDxfId="97"/>
+    <tableColumn id="1" name="Id" dataDxfId="73"/>
+    <tableColumn id="2" name="Name" dataDxfId="72"/>
     <tableColumn id="10" name="Ename"/>
-    <tableColumn id="3" name="Type" dataDxfId="96"/>
+    <tableColumn id="3" name="Type" dataDxfId="71"/>
     <tableColumn id="13" name="SubType"/>
-    <tableColumn id="4" name="Descript" dataDxfId="95"/>
-    <tableColumn id="5" name="Level" dataDxfId="94"/>
-    <tableColumn id="6" name="Rare" dataDxfId="93"/>
-    <tableColumn id="7" name="MaxPile" dataDxfId="92"/>
-    <tableColumn id="8" name="ValueFactor" dataDxfId="91"/>
-    <tableColumn id="11" name="IsUsable" dataDxfId="90"/>
-    <tableColumn id="12" name="IsThrowable" dataDxfId="89"/>
-    <tableColumn id="17" name="ShowCollectTip" dataDxfId="88"/>
+    <tableColumn id="4" name="Descript" dataDxfId="70"/>
+    <tableColumn id="5" name="Level" dataDxfId="69"/>
+    <tableColumn id="6" name="Rare" dataDxfId="68"/>
+    <tableColumn id="7" name="MaxPile" dataDxfId="67"/>
+    <tableColumn id="8" name="ValueFactor" dataDxfId="66"/>
+    <tableColumn id="11" name="IsUsable" dataDxfId="65"/>
+    <tableColumn id="12" name="IsThrowable" dataDxfId="64"/>
+    <tableColumn id="17" name="ShowCollectTip" dataDxfId="63"/>
     <tableColumn id="16" name="RandomGroup"/>
-    <tableColumn id="15" name="Frequency" dataDxfId="87"/>
+    <tableColumn id="15" name="Frequency" dataDxfId="62"/>
     <tableColumn id="9" name="Attributes"/>
-    <tableColumn id="14" name="Url" dataDxfId="86"/>
+    <tableColumn id="14" name="Url" dataDxfId="61"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A3:Q20" totalsRowShown="0" headerRowDxfId="85" dataDxfId="84" tableBorderDxfId="83">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A3:Q20" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48" tableBorderDxfId="47">
   <autoFilter ref="A3:Q20"/>
   <sortState ref="A4:R435">
     <sortCondition ref="A3:A435"/>
   </sortState>
   <tableColumns count="17">
-    <tableColumn id="1" name="Id" dataDxfId="82"/>
-    <tableColumn id="2" name="Name" dataDxfId="81"/>
-    <tableColumn id="10" name="Ename" dataDxfId="80"/>
-    <tableColumn id="3" name="Type" dataDxfId="79"/>
-    <tableColumn id="13" name="SubType" dataDxfId="78"/>
-    <tableColumn id="4" name="Descript" dataDxfId="77"/>
-    <tableColumn id="5" name="Level" dataDxfId="76"/>
-    <tableColumn id="6" name="Rare" dataDxfId="75"/>
-    <tableColumn id="7" name="MaxPile" dataDxfId="74"/>
-    <tableColumn id="8" name="ValueFactor" dataDxfId="73"/>
-    <tableColumn id="11" name="IsUsable" dataDxfId="72"/>
-    <tableColumn id="12" name="IsThrowable" dataDxfId="71"/>
-    <tableColumn id="17" name="ShowCollectTip" dataDxfId="70"/>
-    <tableColumn id="16" name="RandomGroup" dataDxfId="69"/>
-    <tableColumn id="15" name="Frequency" dataDxfId="68"/>
-    <tableColumn id="9" name="Attributes" dataDxfId="67"/>
-    <tableColumn id="14" name="Url" dataDxfId="66"/>
+    <tableColumn id="1" name="Id" dataDxfId="46"/>
+    <tableColumn id="2" name="Name" dataDxfId="45"/>
+    <tableColumn id="10" name="Ename" dataDxfId="44"/>
+    <tableColumn id="3" name="Type" dataDxfId="43"/>
+    <tableColumn id="13" name="SubType" dataDxfId="42"/>
+    <tableColumn id="4" name="Descript" dataDxfId="41"/>
+    <tableColumn id="5" name="Level" dataDxfId="40"/>
+    <tableColumn id="6" name="Rare" dataDxfId="39"/>
+    <tableColumn id="7" name="MaxPile" dataDxfId="38"/>
+    <tableColumn id="8" name="ValueFactor" dataDxfId="37"/>
+    <tableColumn id="11" name="IsUsable" dataDxfId="36"/>
+    <tableColumn id="12" name="IsThrowable" dataDxfId="35"/>
+    <tableColumn id="17" name="ShowCollectTip" dataDxfId="34"/>
+    <tableColumn id="16" name="RandomGroup" dataDxfId="33"/>
+    <tableColumn id="15" name="Frequency" dataDxfId="32"/>
+    <tableColumn id="9" name="Attributes" dataDxfId="31"/>
+    <tableColumn id="14" name="Url" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表1_34" displayName="表1_34" ref="A3:Q121" totalsRowShown="0" headerRowDxfId="65" dataDxfId="64" tableBorderDxfId="63">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表1_34" displayName="表1_34" ref="A3:Q121" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16" tableBorderDxfId="15">
   <autoFilter ref="A3:Q121"/>
   <sortState ref="A4:Q121">
     <sortCondition ref="A3:A121"/>
   </sortState>
   <tableColumns count="17">
-    <tableColumn id="1" name="Id" dataDxfId="62"/>
-    <tableColumn id="2" name="Name" dataDxfId="61"/>
-    <tableColumn id="10" name="Ename" dataDxfId="60"/>
-    <tableColumn id="3" name="Type" dataDxfId="59"/>
-    <tableColumn id="13" name="SubType" dataDxfId="58"/>
-    <tableColumn id="4" name="Descript" dataDxfId="57"/>
-    <tableColumn id="5" name="Level" dataDxfId="56"/>
-    <tableColumn id="6" name="Rare" dataDxfId="55"/>
-    <tableColumn id="7" name="MaxPile" dataDxfId="54"/>
-    <tableColumn id="8" name="ValueFactor" dataDxfId="53"/>
-    <tableColumn id="11" name="IsUsable" dataDxfId="52"/>
-    <tableColumn id="12" name="IsThrowable" dataDxfId="51"/>
+    <tableColumn id="1" name="Id" dataDxfId="14"/>
+    <tableColumn id="2" name="Name" dataDxfId="13"/>
+    <tableColumn id="10" name="Ename" dataDxfId="12"/>
+    <tableColumn id="3" name="Type" dataDxfId="11"/>
+    <tableColumn id="13" name="SubType" dataDxfId="10"/>
+    <tableColumn id="4" name="Descript" dataDxfId="9"/>
+    <tableColumn id="5" name="Level" dataDxfId="8"/>
+    <tableColumn id="6" name="Rare" dataDxfId="7"/>
+    <tableColumn id="7" name="MaxPile" dataDxfId="6"/>
+    <tableColumn id="8" name="ValueFactor" dataDxfId="5"/>
+    <tableColumn id="11" name="IsUsable" dataDxfId="4"/>
+    <tableColumn id="12" name="IsThrowable" dataDxfId="3"/>
     <tableColumn id="17" name="ShowCollectTip"/>
     <tableColumn id="16" name="RandomGroup"/>
-    <tableColumn id="15" name="Frequency" dataDxfId="50"/>
-    <tableColumn id="9" name="Attributes" dataDxfId="49"/>
-    <tableColumn id="14" name="Url" dataDxfId="48"/>
+    <tableColumn id="15" name="Frequency" dataDxfId="2"/>
+    <tableColumn id="9" name="Attributes" dataDxfId="1"/>
+    <tableColumn id="14" name="Url" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9530,10 +9530,10 @@
   <dimension ref="A1:Q352"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B224" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B312" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E241" sqref="E241"/>
+      <selection pane="bottomRight" activeCell="A320" sqref="A320"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -21709,7 +21709,7 @@
     </row>
     <row r="242" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A242" s="20">
-        <v>22110064</v>
+        <v>22110063</v>
       </c>
       <c r="B242" s="43" t="s">
         <v>120</v>
@@ -21759,7 +21759,7 @@
     </row>
     <row r="243" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A243" s="20">
-        <v>22110065</v>
+        <v>22110064</v>
       </c>
       <c r="B243" s="43" t="s">
         <v>192</v>
@@ -21809,7 +21809,7 @@
     </row>
     <row r="244" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A244" s="20">
-        <v>22110066</v>
+        <v>22110065</v>
       </c>
       <c r="B244" s="43" t="s">
         <v>313</v>
@@ -21859,7 +21859,7 @@
     </row>
     <row r="245" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A245" s="20">
-        <v>22110067</v>
+        <v>22110066</v>
       </c>
       <c r="B245" s="40" t="s">
         <v>183</v>
@@ -21909,7 +21909,7 @@
     </row>
     <row r="246" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A246" s="20">
-        <v>22110068</v>
+        <v>22110067</v>
       </c>
       <c r="B246" s="40" t="s">
         <v>185</v>
@@ -21956,7 +21956,7 @@
     </row>
     <row r="247" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A247" s="20">
-        <v>22110069</v>
+        <v>22110068</v>
       </c>
       <c r="B247" s="40" t="s">
         <v>210</v>
@@ -22006,7 +22006,7 @@
     </row>
     <row r="248" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A248" s="20">
-        <v>22110070</v>
+        <v>22110069</v>
       </c>
       <c r="B248" s="40" t="s">
         <v>213</v>
@@ -22056,7 +22056,7 @@
     </row>
     <row r="249" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A249" s="20">
-        <v>22110071</v>
+        <v>22110070</v>
       </c>
       <c r="B249" s="34" t="s">
         <v>129</v>
@@ -22106,7 +22106,7 @@
     </row>
     <row r="250" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A250" s="20">
-        <v>22110072</v>
+        <v>22110071</v>
       </c>
       <c r="B250" s="34" t="s">
         <v>150</v>
@@ -22156,7 +22156,7 @@
     </row>
     <row r="251" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A251" s="20">
-        <v>22110073</v>
+        <v>22110072</v>
       </c>
       <c r="B251" s="34" t="s">
         <v>190</v>
@@ -22206,7 +22206,7 @@
     </row>
     <row r="252" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A252" s="20">
-        <v>22110074</v>
+        <v>22110073</v>
       </c>
       <c r="B252" s="34" t="s">
         <v>202</v>
@@ -22256,7 +22256,7 @@
     </row>
     <row r="253" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A253" s="20">
-        <v>22110075</v>
+        <v>22110074</v>
       </c>
       <c r="B253" s="34" t="s">
         <v>288</v>
@@ -22303,7 +22303,7 @@
     </row>
     <row r="254" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A254" s="20">
-        <v>22110076</v>
+        <v>22110075</v>
       </c>
       <c r="B254" s="34" t="s">
         <v>173</v>
@@ -22353,7 +22353,7 @@
     </row>
     <row r="255" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A255" s="20">
-        <v>22110077</v>
+        <v>22110076</v>
       </c>
       <c r="B255" s="34" t="s">
         <v>208</v>
@@ -22403,7 +22403,7 @@
     </row>
     <row r="256" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A256" s="20">
-        <v>22110078</v>
+        <v>22110077</v>
       </c>
       <c r="B256" s="34" t="s">
         <v>342</v>
@@ -22453,7 +22453,7 @@
     </row>
     <row r="257" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A257" s="20">
-        <v>22110079</v>
+        <v>22110078</v>
       </c>
       <c r="B257" s="39" t="s">
         <v>134</v>
@@ -22503,7 +22503,7 @@
     </row>
     <row r="258" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A258" s="20">
-        <v>22110080</v>
+        <v>22110079</v>
       </c>
       <c r="B258" s="39" t="s">
         <v>180</v>
@@ -22553,7 +22553,7 @@
     </row>
     <row r="259" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A259" s="20">
-        <v>22110081</v>
+        <v>22110080</v>
       </c>
       <c r="B259" s="39" t="s">
         <v>194</v>
@@ -22600,7 +22600,7 @@
     </row>
     <row r="260" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A260" s="20">
-        <v>22110082</v>
+        <v>22110081</v>
       </c>
       <c r="B260" s="39" t="s">
         <v>317</v>
@@ -22647,7 +22647,7 @@
     </row>
     <row r="261" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A261" s="20">
-        <v>22110083</v>
+        <v>22110082</v>
       </c>
       <c r="B261" s="39" t="s">
         <v>1244</v>
@@ -22694,7 +22694,7 @@
     </row>
     <row r="262" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A262" s="20">
-        <v>22110084</v>
+        <v>22110083</v>
       </c>
       <c r="B262" s="39" t="s">
         <v>779</v>
@@ -22741,7 +22741,7 @@
     </row>
     <row r="263" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A263" s="20">
-        <v>22110085</v>
+        <v>22110084</v>
       </c>
       <c r="B263" s="39" t="s">
         <v>218</v>
@@ -22791,7 +22791,7 @@
     </row>
     <row r="264" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A264" s="20">
-        <v>22110086</v>
+        <v>22110085</v>
       </c>
       <c r="B264" s="45" t="s">
         <v>123</v>
@@ -22841,7 +22841,7 @@
     </row>
     <row r="265" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A265" s="20">
-        <v>22110087</v>
+        <v>22110086</v>
       </c>
       <c r="B265" s="45" t="s">
         <v>125</v>
@@ -22891,7 +22891,7 @@
     </row>
     <row r="266" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A266" s="20">
-        <v>22110088</v>
+        <v>22110087</v>
       </c>
       <c r="B266" s="45" t="s">
         <v>110</v>
@@ -22941,7 +22941,7 @@
     </row>
     <row r="267" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A267" s="20">
-        <v>22110089</v>
+        <v>22110088</v>
       </c>
       <c r="B267" s="45" t="s">
         <v>269</v>
@@ -22991,7 +22991,7 @@
     </row>
     <row r="268" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A268" s="20">
-        <v>22110090</v>
+        <v>22110089</v>
       </c>
       <c r="B268" s="45" t="s">
         <v>277</v>
@@ -23041,7 +23041,7 @@
     </row>
     <row r="269" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A269" s="20">
-        <v>22110091</v>
+        <v>22110090</v>
       </c>
       <c r="B269" s="45" t="s">
         <v>802</v>
@@ -23091,7 +23091,7 @@
     </row>
     <row r="270" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A270" s="20">
-        <v>22110092</v>
+        <v>22110091</v>
       </c>
       <c r="B270" s="46" t="s">
         <v>251</v>
@@ -23141,7 +23141,7 @@
     </row>
     <row r="271" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A271" s="20">
-        <v>22110093</v>
+        <v>22110092</v>
       </c>
       <c r="B271" s="46" t="s">
         <v>55</v>
@@ -23188,7 +23188,7 @@
     </row>
     <row r="272" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A272" s="20">
-        <v>22110094</v>
+        <v>22110093</v>
       </c>
       <c r="B272" s="46" t="s">
         <v>281</v>
@@ -23235,7 +23235,7 @@
     </row>
     <row r="273" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A273" s="20">
-        <v>22110095</v>
+        <v>22110094</v>
       </c>
       <c r="B273" s="46" t="s">
         <v>322</v>
@@ -23282,7 +23282,7 @@
     </row>
     <row r="274" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A274" s="20">
-        <v>22110096</v>
+        <v>22110095</v>
       </c>
       <c r="B274" s="46" t="s">
         <v>283</v>
@@ -23329,7 +23329,7 @@
     </row>
     <row r="275" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A275" s="20">
-        <v>22110097</v>
+        <v>22110096</v>
       </c>
       <c r="B275" s="47" t="s">
         <v>273</v>
@@ -23379,7 +23379,7 @@
     </row>
     <row r="276" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A276" s="20">
-        <v>22110098</v>
+        <v>22110097</v>
       </c>
       <c r="B276" s="47" t="s">
         <v>275</v>
@@ -23429,7 +23429,7 @@
     </row>
     <row r="277" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A277" s="20">
-        <v>22110099</v>
+        <v>22110098</v>
       </c>
       <c r="B277" s="47" t="s">
         <v>295</v>
@@ -23476,7 +23476,7 @@
     </row>
     <row r="278" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A278" s="20">
-        <v>22110100</v>
+        <v>22110099</v>
       </c>
       <c r="B278" s="47" t="s">
         <v>297</v>
@@ -23526,7 +23526,7 @@
     </row>
     <row r="279" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A279" s="20">
-        <v>22110101</v>
+        <v>22110100</v>
       </c>
       <c r="B279" s="47" t="s">
         <v>299</v>
@@ -23576,7 +23576,7 @@
     </row>
     <row r="280" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A280" s="20">
-        <v>22110102</v>
+        <v>22110101</v>
       </c>
       <c r="B280" s="47" t="s">
         <v>329</v>
@@ -23626,7 +23626,7 @@
     </row>
     <row r="281" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A281" s="20">
-        <v>22110103</v>
+        <v>22110102</v>
       </c>
       <c r="B281" s="47" t="s">
         <v>333</v>
@@ -23676,7 +23676,7 @@
     </row>
     <row r="282" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A282" s="20">
-        <v>22110104</v>
+        <v>22110103</v>
       </c>
       <c r="B282" s="47" t="s">
         <v>335</v>
@@ -23726,7 +23726,7 @@
     </row>
     <row r="283" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A283" s="20">
-        <v>22110105</v>
+        <v>22110104</v>
       </c>
       <c r="B283" s="47" t="s">
         <v>302</v>
@@ -23776,7 +23776,7 @@
     </row>
     <row r="284" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A284" s="20">
-        <v>22110106</v>
+        <v>22110105</v>
       </c>
       <c r="B284" s="47" t="s">
         <v>787</v>
@@ -23826,7 +23826,7 @@
     </row>
     <row r="285" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A285" s="20">
-        <v>22110107</v>
+        <v>22110106</v>
       </c>
       <c r="B285" s="47" t="s">
         <v>798</v>
@@ -23876,7 +23876,7 @@
     </row>
     <row r="286" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A286" s="20">
-        <v>22110108</v>
+        <v>22110107</v>
       </c>
       <c r="B286" s="47" t="s">
         <v>784</v>
@@ -23973,7 +23973,7 @@
     </row>
     <row r="288" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A288" s="20">
-        <v>22110108</v>
+        <v>22110109</v>
       </c>
       <c r="B288" s="47" t="s">
         <v>224</v>
@@ -24023,7 +24023,7 @@
     </row>
     <row r="289" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A289" s="20">
-        <v>22110108</v>
+        <v>22110110</v>
       </c>
       <c r="B289" s="47" t="s">
         <v>226</v>
@@ -24073,7 +24073,7 @@
     </row>
     <row r="290" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A290" s="20">
-        <v>22110108</v>
+        <v>22110111</v>
       </c>
       <c r="B290" s="47" t="s">
         <v>229</v>
@@ -24123,7 +24123,7 @@
     </row>
     <row r="291" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A291" s="20">
-        <v>22110108</v>
+        <v>22110112</v>
       </c>
       <c r="B291" s="47" t="s">
         <v>232</v>
@@ -24173,7 +24173,7 @@
     </row>
     <row r="292" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A292" s="20">
-        <v>22110108</v>
+        <v>22110113</v>
       </c>
       <c r="B292" s="47" t="s">
         <v>235</v>
@@ -24223,7 +24223,7 @@
     </row>
     <row r="293" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A293" s="20">
-        <v>22110108</v>
+        <v>22110114</v>
       </c>
       <c r="B293" s="47" t="s">
         <v>238</v>
@@ -24273,7 +24273,7 @@
     </row>
     <row r="294" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A294" s="20">
-        <v>22110108</v>
+        <v>22110115</v>
       </c>
       <c r="B294" s="47" t="s">
         <v>241</v>
@@ -24323,7 +24323,7 @@
     </row>
     <row r="295" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A295" s="20">
-        <v>22110108</v>
+        <v>22110116</v>
       </c>
       <c r="B295" s="47" t="s">
         <v>244</v>
@@ -24373,7 +24373,7 @@
     </row>
     <row r="296" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A296" s="20">
-        <v>22110108</v>
+        <v>22110117</v>
       </c>
       <c r="B296" s="47" t="s">
         <v>147</v>
@@ -24423,7 +24423,7 @@
     </row>
     <row r="297" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A297" s="20">
-        <v>22110109</v>
+        <v>22110118</v>
       </c>
       <c r="B297" s="44" t="s">
         <v>344</v>
@@ -24473,7 +24473,7 @@
     </row>
     <row r="298" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A298" s="20">
-        <v>22110110</v>
+        <v>22110119</v>
       </c>
       <c r="B298" s="44" t="s">
         <v>347</v>
@@ -24523,7 +24523,7 @@
     </row>
     <row r="299" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A299" s="20">
-        <v>22110111</v>
+        <v>22110120</v>
       </c>
       <c r="B299" s="44" t="s">
         <v>220</v>
@@ -24573,7 +24573,7 @@
     </row>
     <row r="300" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A300" s="20">
-        <v>22110112</v>
+        <v>22110121</v>
       </c>
       <c r="B300" s="44" t="s">
         <v>117</v>
@@ -24623,7 +24623,7 @@
     </row>
     <row r="301" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A301" s="20">
-        <v>22110113</v>
+        <v>22110122</v>
       </c>
       <c r="B301" s="44" t="s">
         <v>114</v>
@@ -24673,7 +24673,7 @@
     </row>
     <row r="302" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A302" s="20">
-        <v>22110114</v>
+        <v>22110123</v>
       </c>
       <c r="B302" s="44" t="s">
         <v>337</v>
@@ -24723,7 +24723,7 @@
     </row>
     <row r="303" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A303" s="20">
-        <v>22110115</v>
+        <v>22110124</v>
       </c>
       <c r="B303" s="44" t="s">
         <v>74</v>
@@ -24773,7 +24773,7 @@
     </row>
     <row r="304" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A304" s="20">
-        <v>22110116</v>
+        <v>22110125</v>
       </c>
       <c r="B304" s="44" t="s">
         <v>53</v>
@@ -24823,7 +24823,7 @@
     </row>
     <row r="305" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A305" s="20">
-        <v>22110117</v>
+        <v>22110126</v>
       </c>
       <c r="B305" s="44" t="s">
         <v>782</v>
@@ -24873,7 +24873,7 @@
     </row>
     <row r="306" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A306" s="20">
-        <v>22110118</v>
+        <v>22110127</v>
       </c>
       <c r="B306" s="44" t="s">
         <v>102</v>
@@ -24923,7 +24923,7 @@
     </row>
     <row r="307" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A307" s="20">
-        <v>22110119</v>
+        <v>22110128</v>
       </c>
       <c r="B307" s="44" t="s">
         <v>105</v>
@@ -25173,7 +25173,7 @@
     </row>
     <row r="312" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A312" s="20">
-        <v>22110134</v>
+        <v>22110133</v>
       </c>
       <c r="B312" s="20" t="s">
         <v>205</v>
@@ -25223,7 +25223,7 @@
     </row>
     <row r="313" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A313" s="20">
-        <v>22110135</v>
+        <v>22110134</v>
       </c>
       <c r="B313" s="20" t="s">
         <v>59</v>
@@ -25270,7 +25270,7 @@
     </row>
     <row r="314" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A314" s="20">
-        <v>22110136</v>
+        <v>22110135</v>
       </c>
       <c r="B314" s="20" t="s">
         <v>291</v>
@@ -25320,7 +25320,7 @@
     </row>
     <row r="315" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A315" s="20">
-        <v>22110137</v>
+        <v>22110136</v>
       </c>
       <c r="B315" s="20" t="s">
         <v>167</v>
@@ -25370,7 +25370,7 @@
     </row>
     <row r="316" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A316" s="20">
-        <v>22110138</v>
+        <v>22110137</v>
       </c>
       <c r="B316" s="20" t="s">
         <v>169</v>
@@ -25420,7 +25420,7 @@
     </row>
     <row r="317" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A317" s="20">
-        <v>22110139</v>
+        <v>22110138</v>
       </c>
       <c r="B317" s="20" t="s">
         <v>171</v>
@@ -25470,7 +25470,7 @@
     </row>
     <row r="318" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A318" s="20">
-        <v>22110140</v>
+        <v>22110139</v>
       </c>
       <c r="B318" s="20" t="s">
         <v>311</v>
@@ -25520,7 +25520,7 @@
     </row>
     <row r="319" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A319" s="20">
-        <v>22110141</v>
+        <v>22110140</v>
       </c>
       <c r="B319" s="20" t="s">
         <v>320</v>
@@ -25567,7 +25567,7 @@
     </row>
     <row r="320" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A320" s="20">
-        <v>22110142</v>
+        <v>22110141</v>
       </c>
       <c r="B320" s="20" t="s">
         <v>324</v>
@@ -25617,7 +25617,7 @@
     </row>
     <row r="321" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A321" s="20">
-        <v>22110143</v>
+        <v>22110142</v>
       </c>
       <c r="B321" s="20" t="s">
         <v>773</v>
@@ -25667,7 +25667,7 @@
     </row>
     <row r="322" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A322" s="20">
-        <v>22110144</v>
+        <v>22110143</v>
       </c>
       <c r="B322" s="20" t="s">
         <v>793</v>
@@ -25717,7 +25717,7 @@
     </row>
     <row r="323" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A323" s="20">
-        <v>22110145</v>
+        <v>22110144</v>
       </c>
       <c r="B323" s="20" t="s">
         <v>796</v>
@@ -25764,7 +25764,7 @@
     </row>
     <row r="324" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A324" s="20">
-        <v>22110146</v>
+        <v>22110145</v>
       </c>
       <c r="B324" s="20" t="s">
         <v>764</v>
@@ -25811,7 +25811,7 @@
     </row>
     <row r="325" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A325" s="20">
-        <v>22110147</v>
+        <v>22110146</v>
       </c>
       <c r="B325" s="20" t="s">
         <v>767</v>
@@ -27155,109 +27155,109 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="B4:Q29 B41:Q352">
-    <cfRule type="containsBlanks" dxfId="47" priority="25">
+    <cfRule type="containsBlanks" dxfId="101" priority="25">
       <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H29 H41:H352">
-    <cfRule type="cellIs" dxfId="46" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="20" operator="equal">
       <formula>7</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="21" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="22" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="23" operator="between">
+    <cfRule type="cellIs" dxfId="97" priority="23" operator="between">
       <formula>3</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="24" operator="between">
+    <cfRule type="cellIs" dxfId="96" priority="24" operator="between">
       <formula>1</formula>
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B30:Q31 G32:Q32 B32:E40 I33:Q37 I39:Q40 I38:O38 Q38">
-    <cfRule type="containsBlanks" dxfId="41" priority="19">
+    <cfRule type="containsBlanks" dxfId="95" priority="19">
       <formula>LEN(TRIM(B30))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H30:H32">
-    <cfRule type="cellIs" dxfId="40" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="14" operator="equal">
       <formula>7</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="15" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="16" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="17" operator="between">
+    <cfRule type="cellIs" dxfId="91" priority="17" operator="between">
       <formula>3</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="18" operator="between">
+    <cfRule type="cellIs" dxfId="90" priority="18" operator="between">
       <formula>1</formula>
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F32">
-    <cfRule type="containsBlanks" dxfId="35" priority="13">
+    <cfRule type="containsBlanks" dxfId="89" priority="13">
       <formula>LEN(TRIM(F32))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F33:H33 G34:H40">
-    <cfRule type="containsBlanks" dxfId="34" priority="12">
+    <cfRule type="containsBlanks" dxfId="88" priority="12">
       <formula>LEN(TRIM(F33))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33:H40">
-    <cfRule type="cellIs" dxfId="33" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="7" operator="equal">
       <formula>7</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="8" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="9" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="10" operator="between">
+    <cfRule type="cellIs" dxfId="84" priority="10" operator="between">
       <formula>3</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="11" operator="between">
+    <cfRule type="cellIs" dxfId="83" priority="11" operator="between">
       <formula>1</formula>
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F34">
-    <cfRule type="containsBlanks" dxfId="28" priority="6">
+    <cfRule type="containsBlanks" dxfId="82" priority="6">
       <formula>LEN(TRIM(F34))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F35:F37">
-    <cfRule type="containsBlanks" dxfId="27" priority="5">
+    <cfRule type="containsBlanks" dxfId="81" priority="5">
       <formula>LEN(TRIM(F35))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F38">
-    <cfRule type="containsBlanks" dxfId="26" priority="4">
+    <cfRule type="containsBlanks" dxfId="80" priority="4">
       <formula>LEN(TRIM(F38))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F39">
-    <cfRule type="containsBlanks" dxfId="25" priority="3">
+    <cfRule type="containsBlanks" dxfId="79" priority="3">
       <formula>LEN(TRIM(F39))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F40">
-    <cfRule type="containsBlanks" dxfId="24" priority="2">
+    <cfRule type="containsBlanks" dxfId="78" priority="2">
       <formula>LEN(TRIM(F40))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P38">
-    <cfRule type="containsBlanks" dxfId="23" priority="1">
+    <cfRule type="containsBlanks" dxfId="77" priority="1">
       <formula>LEN(TRIM(P38))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -28091,50 +28091,50 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="B6:Q20 B5:D5 L5:P5 F5:J5">
-    <cfRule type="containsBlanks" dxfId="22" priority="12">
+    <cfRule type="containsBlanks" dxfId="60" priority="12">
       <formula>LEN(TRIM(B5))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:G4 I4:Q4">
-    <cfRule type="containsBlanks" dxfId="21" priority="10">
+    <cfRule type="containsBlanks" dxfId="59" priority="10">
       <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q5">
-    <cfRule type="containsBlanks" dxfId="20" priority="9">
+    <cfRule type="containsBlanks" dxfId="58" priority="9">
       <formula>LEN(TRIM(Q5))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="containsBlanks" dxfId="19" priority="8">
+    <cfRule type="containsBlanks" dxfId="57" priority="8">
       <formula>LEN(TRIM(K5))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="containsBlanks" dxfId="18" priority="7">
+    <cfRule type="containsBlanks" dxfId="56" priority="7">
       <formula>LEN(TRIM(E5))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H20">
-    <cfRule type="containsBlanks" dxfId="17" priority="6">
+    <cfRule type="containsBlanks" dxfId="55" priority="6">
       <formula>LEN(TRIM(H4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H20">
-    <cfRule type="cellIs" dxfId="16" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="1" operator="equal">
       <formula>7</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="2" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="3" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="4" operator="between">
+    <cfRule type="cellIs" dxfId="51" priority="4" operator="between">
       <formula>3</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="50" priority="5" operator="between">
       <formula>1</formula>
       <formula>2</formula>
     </cfRule>
@@ -33123,55 +33123,55 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="J97:J113 F109:J114 F9:J11 J5:J21 O8:P21 E5:J8 E115:J121 K5:P7 K8:N37 E4:G4 E88:J108 K88:Q121 Q5:Q73 K38:P73 E12:J73 E80:Q87 I4:Q4">
-    <cfRule type="containsBlanks" dxfId="11" priority="15">
+    <cfRule type="containsBlanks" dxfId="29" priority="15">
       <formula>LEN(TRIM(E4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E109:E111">
-    <cfRule type="containsBlanks" dxfId="10" priority="13">
+    <cfRule type="containsBlanks" dxfId="28" priority="13">
       <formula>LEN(TRIM(E109))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E112:E114">
-    <cfRule type="containsBlanks" dxfId="9" priority="12">
+    <cfRule type="containsBlanks" dxfId="27" priority="12">
       <formula>LEN(TRIM(E112))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9:E11">
-    <cfRule type="containsBlanks" dxfId="8" priority="11">
+    <cfRule type="containsBlanks" dxfId="26" priority="11">
       <formula>LEN(TRIM(E9))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J22:J37 O22:P37">
-    <cfRule type="containsBlanks" dxfId="7" priority="10">
+    <cfRule type="containsBlanks" dxfId="25" priority="10">
       <formula>LEN(TRIM(J22))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E74:Q79">
-    <cfRule type="containsBlanks" dxfId="6" priority="7">
+    <cfRule type="containsBlanks" dxfId="24" priority="7">
       <formula>LEN(TRIM(E74))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H121">
-    <cfRule type="containsBlanks" dxfId="5" priority="6">
+    <cfRule type="containsBlanks" dxfId="23" priority="6">
       <formula>LEN(TRIM(H4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H121">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="1" operator="equal">
       <formula>7</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="2" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="3" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="between">
+    <cfRule type="cellIs" dxfId="19" priority="4" operator="between">
       <formula>3</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="18" priority="5" operator="between">
       <formula>1</formula>
       <formula>2</formula>
     </cfRule>

</xml_diff>

<commit_message>
new click label color show effect
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/HItem.xlsx
+++ b/ConfigData/Xlsx/HItem.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView minimized="1" xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="材料" sheetId="1" r:id="rId1"/>
@@ -9108,6 +9108,74 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -9214,7 +9282,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="C7EDCC"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -9530,10 +9598,10 @@
   <dimension ref="A1:Q352"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B312" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B59" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A320" sqref="A320"/>
+      <selection pane="bottomRight" activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
optimise the tip of gift package
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/HItem.xlsx
+++ b/ConfigData/Xlsx/HItem.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -217,7 +217,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3422" uniqueCount="1818">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3421" uniqueCount="1818">
   <si>
     <t>血蓟</t>
   </si>
@@ -28173,7 +28173,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -28363,9 +28363,6 @@
       </c>
       <c r="E4">
         <v>12</v>
-      </c>
-      <c r="F4" t="s">
-        <v>631</v>
       </c>
       <c r="G4">
         <v>1</v>

</xml_diff>